<commit_message>
Adding opCode BIts in table
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aca51a41c02ca2ab/Documents/GitHub/Architecture-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\CCE\Year 3 - Senior 1\Semester 2\Arch\Project\Repo\Architecture-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{5B46B3C9-9EED-4C51-86C2-2B59B18A328C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59303F2D-DB62-4D70-BBE1-8B055206C0BD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D7FDEE-5691-42E0-BBBD-C1C73786C545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0E858663-1FD8-418A-96F6-784D0D9CF43C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="114">
   <si>
     <t>Instruction</t>
   </si>
@@ -283,9 +283,6 @@
     <t>"01"</t>
   </si>
   <si>
-    <t>OpCode (5)</t>
-  </si>
-  <si>
     <t>Rs1 (3)</t>
   </si>
   <si>
@@ -374,6 +371,15 @@
   </si>
   <si>
     <t>"100011"</t>
+  </si>
+  <si>
+    <t>OpCode (6)</t>
+  </si>
+  <si>
+    <t>2Bits (Type of Instruction)</t>
+  </si>
+  <si>
+    <t>4Bits (Number of instruction in this type)</t>
   </si>
 </sst>
 </file>
@@ -561,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -584,12 +590,84 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -602,76 +680,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -988,10 +1006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9834DC43-CD6B-4773-9F5D-9D470392FD57}">
-  <dimension ref="A1:AU37"/>
+  <dimension ref="A1:AX37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T32" sqref="T32"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AU8" sqref="AU8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1026,246 +1044,259 @@
     <col min="41" max="41" width="11.5546875" customWidth="1"/>
     <col min="42" max="42" width="16.6640625" customWidth="1"/>
     <col min="47" max="47" width="12.88671875" customWidth="1"/>
+    <col min="49" max="49" width="22.33203125" customWidth="1"/>
+    <col min="50" max="50" width="37.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="83.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:50" ht="83.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="19"/>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="23"/>
       <c r="S1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="T1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="U1" s="17" t="s">
+      <c r="U1" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="V1" s="18"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="17" t="s">
+      <c r="V1" s="22"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="17" t="s">
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="37"/>
-      <c r="AE1" s="8" t="s">
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AF1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="AH1" s="11" t="s">
+      <c r="AH1" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="13"/>
-      <c r="AM1" s="11" t="s">
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="36"/>
+      <c r="AK1" s="37"/>
+      <c r="AM1" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="AN1" s="12"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="13"/>
-      <c r="AR1" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="AS1" s="12"/>
-      <c r="AT1" s="12"/>
-      <c r="AU1" s="13"/>
-    </row>
-    <row r="2" spans="1:47" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+      <c r="AN1" s="36"/>
+      <c r="AO1" s="36"/>
+      <c r="AP1" s="37"/>
+      <c r="AR1" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="AS1" s="36"/>
+      <c r="AT1" s="36"/>
+      <c r="AU1" s="37"/>
+      <c r="AW1" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="AX1" s="36"/>
+    </row>
+    <row r="2" spans="1:50" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="23" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="L2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="23" t="s">
+      <c r="M2" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="23" t="s">
+      <c r="N2" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="O2" s="23" t="s">
+      <c r="O2" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="P2" s="23" t="s">
+      <c r="P2" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14" t="s">
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="T2" s="14" t="s">
+      <c r="T2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="14" t="s">
+      <c r="U2" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="V2" s="14" t="s">
+      <c r="V2" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="W2" s="14" t="s">
+      <c r="W2" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="X2" s="14" t="s">
+      <c r="X2" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="Y2" s="14" t="s">
+      <c r="Y2" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="Z2" s="14" t="s">
+      <c r="Z2" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="AA2" s="14" t="s">
+      <c r="AA2" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="AB2" s="14" t="s">
+      <c r="AB2" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="AC2" s="14" t="s">
+      <c r="AC2" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="36" t="s">
+      <c r="AD2" s="14"/>
+      <c r="AE2" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AF2" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="AH2" s="10" t="s">
+      <c r="AH2" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="AI2" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AK2" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AM2" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP2" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AM2" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="AP2" s="3" t="s">
+      <c r="AR2" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="AS2" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="AR2" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="AS2" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="AT2" s="21"/>
-      <c r="AU2" s="22"/>
-    </row>
-    <row r="3" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="15"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15"/>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="15"/>
-      <c r="Z3" s="15"/>
-      <c r="AA3" s="15"/>
-      <c r="AB3" s="15"/>
-      <c r="AC3" s="15"/>
-      <c r="AD3" s="37"/>
-      <c r="AE3" s="36" t="s">
+      <c r="AT2" s="38"/>
+      <c r="AU2" s="20"/>
+      <c r="AV2" s="41"/>
+      <c r="AW2" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AX2" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:50" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="16"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="16"/>
+      <c r="Y3" s="16"/>
+      <c r="Z3" s="16"/>
+      <c r="AA3" s="16"/>
+      <c r="AB3" s="16"/>
+      <c r="AC3" s="16"/>
+      <c r="AD3" s="14"/>
+      <c r="AE3" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="AF3" s="4" t="s">
+      <c r="AF3" s="12" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:47" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:50" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="20">
-        <v>0</v>
-      </c>
-      <c r="C4" s="22"/>
+      <c r="B4" s="19">
+        <v>0</v>
+      </c>
+      <c r="C4" s="20"/>
       <c r="D4" s="2">
         <v>0</v>
       </c>
@@ -1307,31 +1338,31 @@
       </c>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
-      <c r="AA4" s="9"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="37"/>
-      <c r="AE4" s="36" t="s">
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
+      <c r="AD4" s="14"/>
+      <c r="AE4" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="AF4" s="4" t="s">
+      <c r="AF4" s="12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:47" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:50" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="22"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1349,33 +1380,33 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
       <c r="W5" s="4"/>
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
       <c r="Z5" s="4"/>
-      <c r="AA5" s="9"/>
-      <c r="AB5" s="9"/>
-      <c r="AC5" s="9"/>
-      <c r="AD5" s="37"/>
-      <c r="AE5" s="36" t="s">
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="8"/>
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="AF5" s="4" t="s">
+      <c r="AF5" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:47" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:50" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="20">
-        <v>0</v>
-      </c>
-      <c r="C6" s="22"/>
+      <c r="B6" s="19">
+        <v>0</v>
+      </c>
+      <c r="C6" s="20"/>
       <c r="D6" s="2">
         <v>0</v>
       </c>
@@ -1420,8 +1451,8 @@
       <c r="S6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T6" s="10" t="s">
-        <v>92</v>
+      <c r="T6" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="U6" s="4" t="s">
         <v>61</v>
@@ -1435,25 +1466,25 @@
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
       <c r="Z6" s="4"/>
-      <c r="AA6" s="9"/>
-      <c r="AB6" s="9"/>
-      <c r="AC6" s="9"/>
-      <c r="AD6" s="37"/>
-      <c r="AE6" s="36" t="s">
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="14"/>
+      <c r="AE6" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="AF6" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:47" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AF6" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:50" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="20">
-        <v>1</v>
-      </c>
-      <c r="C7" s="22"/>
+      <c r="B7" s="19">
+        <v>1</v>
+      </c>
+      <c r="C7" s="20"/>
       <c r="D7" s="2">
         <v>0</v>
       </c>
@@ -1499,7 +1530,7 @@
         <v>17</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="U7" s="4" t="s">
         <v>61</v>
@@ -1513,25 +1544,25 @@
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
       <c r="Z7" s="4"/>
-      <c r="AA7" s="9"/>
-      <c r="AB7" s="9"/>
-      <c r="AC7" s="9"/>
-      <c r="AD7" s="37"/>
-      <c r="AE7" s="36" t="s">
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="14"/>
+      <c r="AE7" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="AF7" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:47" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AF7" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:50" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="20">
-        <v>1</v>
-      </c>
-      <c r="C8" s="22"/>
+      <c r="B8" s="19">
+        <v>1</v>
+      </c>
+      <c r="C8" s="20"/>
       <c r="D8" s="2">
         <v>0</v>
       </c>
@@ -1576,8 +1607,8 @@
       <c r="S8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T8" s="9" t="s">
-        <v>94</v>
+      <c r="T8" s="8" t="s">
+        <v>93</v>
       </c>
       <c r="U8" s="4" t="s">
         <v>61</v>
@@ -1591,25 +1622,25 @@
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
       <c r="Z8" s="4"/>
-      <c r="AA8" s="9"/>
-      <c r="AB8" s="9"/>
-      <c r="AC8" s="9"/>
-      <c r="AD8" s="37"/>
-      <c r="AE8" s="36" t="s">
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="14"/>
+      <c r="AE8" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="AF8" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:47" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AF8" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:50" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="20">
-        <v>0</v>
-      </c>
-      <c r="C9" s="22"/>
+      <c r="B9" s="19">
+        <v>0</v>
+      </c>
+      <c r="C9" s="20"/>
       <c r="D9" s="2">
         <v>0</v>
       </c>
@@ -1654,8 +1685,8 @@
       <c r="S9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T9" s="9" t="s">
-        <v>95</v>
+      <c r="T9" s="8" t="s">
+        <v>94</v>
       </c>
       <c r="U9" s="4" t="s">
         <v>58</v>
@@ -1669,25 +1700,25 @@
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
       <c r="Z9" s="4"/>
-      <c r="AA9" s="9"/>
-      <c r="AB9" s="9"/>
-      <c r="AC9" s="9"/>
-      <c r="AD9" s="37"/>
-      <c r="AE9" s="36" t="s">
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="14"/>
+      <c r="AE9" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="AF9" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:47" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AF9" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:50" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="20">
-        <v>1</v>
-      </c>
-      <c r="C10" s="22"/>
+      <c r="B10" s="19">
+        <v>1</v>
+      </c>
+      <c r="C10" s="20"/>
       <c r="D10" s="2">
         <v>0</v>
       </c>
@@ -1732,8 +1763,8 @@
       <c r="S10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T10" s="9" t="s">
-        <v>96</v>
+      <c r="T10" s="8" t="s">
+        <v>95</v>
       </c>
       <c r="U10" s="4" t="s">
         <v>61</v>
@@ -1747,19 +1778,19 @@
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
       <c r="Z10" s="4"/>
-      <c r="AA10" s="9"/>
-      <c r="AB10" s="9"/>
-      <c r="AC10" s="9"/>
-      <c r="AD10" s="35"/>
-    </row>
-    <row r="11" spans="1:47" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="8"/>
+      <c r="AD10" s="13"/>
+    </row>
+    <row r="11" spans="1:50" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="20">
-        <v>1</v>
-      </c>
-      <c r="C11" s="22"/>
+      <c r="B11" s="19">
+        <v>1</v>
+      </c>
+      <c r="C11" s="20"/>
       <c r="D11" s="2">
         <v>0</v>
       </c>
@@ -1804,8 +1835,8 @@
       <c r="S11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T11" s="9" t="s">
-        <v>97</v>
+      <c r="T11" s="8" t="s">
+        <v>96</v>
       </c>
       <c r="U11" s="4" t="s">
         <v>62</v>
@@ -1819,19 +1850,19 @@
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
       <c r="Z11" s="4"/>
-      <c r="AA11" s="9"/>
-      <c r="AB11" s="9"/>
-      <c r="AC11" s="9"/>
-      <c r="AD11" s="35"/>
-    </row>
-    <row r="12" spans="1:47" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
+      <c r="AC11" s="8"/>
+      <c r="AD11" s="13"/>
+    </row>
+    <row r="12" spans="1:50" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="20">
-        <v>1</v>
-      </c>
-      <c r="C12" s="22"/>
+      <c r="B12" s="19">
+        <v>1</v>
+      </c>
+      <c r="C12" s="20"/>
       <c r="D12" s="2">
         <v>1</v>
       </c>
@@ -1876,8 +1907,8 @@
       <c r="S12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T12" s="9" t="s">
-        <v>98</v>
+      <c r="T12" s="8" t="s">
+        <v>97</v>
       </c>
       <c r="U12" s="4" t="s">
         <v>62</v>
@@ -1891,435 +1922,435 @@
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
       <c r="Z12" s="4"/>
-      <c r="AA12" s="9"/>
-      <c r="AB12" s="9"/>
-      <c r="AC12" s="9"/>
-      <c r="AD12" s="35"/>
-    </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A13" s="33" t="s">
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="8"/>
+      <c r="AC12" s="8"/>
+      <c r="AD12" s="13"/>
+    </row>
+    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="29">
-        <v>1</v>
-      </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="14">
-        <v>0</v>
-      </c>
-      <c r="E13" s="14">
-        <v>0</v>
-      </c>
-      <c r="F13" s="14">
-        <v>0</v>
-      </c>
-      <c r="G13" s="14">
-        <v>0</v>
-      </c>
-      <c r="H13" s="14">
-        <v>0</v>
-      </c>
-      <c r="I13" s="14">
+      <c r="B13" s="24">
+        <v>1</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="15">
+        <v>0</v>
+      </c>
+      <c r="E13" s="15">
+        <v>0</v>
+      </c>
+      <c r="F13" s="15">
+        <v>0</v>
+      </c>
+      <c r="G13" s="15">
+        <v>0</v>
+      </c>
+      <c r="H13" s="15">
+        <v>0</v>
+      </c>
+      <c r="I13" s="15">
         <v>101</v>
       </c>
-      <c r="J13" s="14" t="s">
+      <c r="J13" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="K13" s="14">
-        <v>0</v>
-      </c>
-      <c r="L13" s="14">
-        <v>0</v>
-      </c>
-      <c r="M13" s="14">
-        <v>0</v>
-      </c>
-      <c r="N13" s="14">
-        <v>0</v>
-      </c>
-      <c r="O13" s="14">
-        <v>1</v>
-      </c>
-      <c r="P13" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14" t="s">
+      <c r="K13" s="15">
+        <v>0</v>
+      </c>
+      <c r="L13" s="15">
+        <v>0</v>
+      </c>
+      <c r="M13" s="15">
+        <v>0</v>
+      </c>
+      <c r="N13" s="15">
+        <v>0</v>
+      </c>
+      <c r="O13" s="15">
+        <v>1</v>
+      </c>
+      <c r="P13" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="T13" s="14" t="s">
+      <c r="T13" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="U13" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="V13" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="W13" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="15"/>
+      <c r="AD13" s="13"/>
+    </row>
+    <row r="14" spans="1:50" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="18"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="16"/>
+      <c r="W14" s="16"/>
+      <c r="X14" s="16"/>
+      <c r="Y14" s="16"/>
+      <c r="Z14" s="16"/>
+      <c r="AA14" s="16"/>
+      <c r="AB14" s="16"/>
+      <c r="AC14" s="16"/>
+      <c r="AD14" s="13"/>
+    </row>
+    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="24">
+        <v>1</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="15">
+        <v>0</v>
+      </c>
+      <c r="F15" s="15">
+        <v>0</v>
+      </c>
+      <c r="G15" s="15">
+        <v>0</v>
+      </c>
+      <c r="H15" s="15">
+        <v>0</v>
+      </c>
+      <c r="I15" s="15">
+        <v>100</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="K15" s="15">
+        <v>0</v>
+      </c>
+      <c r="L15" s="15">
+        <v>0</v>
+      </c>
+      <c r="M15" s="15">
+        <v>0</v>
+      </c>
+      <c r="N15" s="15">
+        <v>0</v>
+      </c>
+      <c r="O15" s="15">
+        <v>1</v>
+      </c>
+      <c r="P15" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="T15" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="U13" s="14" t="s">
+      <c r="U15" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="V13" s="14" t="s">
+      <c r="V15" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="W13" s="14" t="s">
+      <c r="W15" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="X13" s="14"/>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="14"/>
-      <c r="AA13" s="14"/>
-      <c r="AB13" s="14"/>
-      <c r="AC13" s="14"/>
-      <c r="AD13" s="35"/>
-    </row>
-    <row r="14" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="34"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="15"/>
-      <c r="Z14" s="15"/>
-      <c r="AA14" s="15"/>
-      <c r="AB14" s="15"/>
-      <c r="AC14" s="15"/>
-      <c r="AD14" s="35"/>
-    </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A15" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="29">
-        <v>1</v>
-      </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="14">
-        <v>0</v>
-      </c>
-      <c r="E15" s="14">
-        <v>0</v>
-      </c>
-      <c r="F15" s="14">
-        <v>0</v>
-      </c>
-      <c r="G15" s="14">
-        <v>0</v>
-      </c>
-      <c r="H15" s="14">
-        <v>0</v>
-      </c>
-      <c r="I15" s="14">
+      <c r="X15" s="15"/>
+      <c r="Y15" s="15"/>
+      <c r="Z15" s="15"/>
+      <c r="AA15" s="15"/>
+      <c r="AB15" s="15"/>
+      <c r="AC15" s="15"/>
+      <c r="AD15" s="13"/>
+    </row>
+    <row r="16" spans="1:50" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="18"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
+      <c r="V16" s="16"/>
+      <c r="W16" s="16"/>
+      <c r="X16" s="16"/>
+      <c r="Y16" s="16"/>
+      <c r="Z16" s="16"/>
+      <c r="AA16" s="16"/>
+      <c r="AB16" s="16"/>
+      <c r="AC16" s="16"/>
+      <c r="AD16" s="13"/>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="24">
+        <v>1</v>
+      </c>
+      <c r="C17" s="25"/>
+      <c r="D17" s="15">
+        <v>0</v>
+      </c>
+      <c r="E17" s="15">
+        <v>0</v>
+      </c>
+      <c r="F17" s="15">
+        <v>0</v>
+      </c>
+      <c r="G17" s="15">
+        <v>0</v>
+      </c>
+      <c r="H17" s="15">
+        <v>0</v>
+      </c>
+      <c r="I17" s="15">
+        <v>111</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="K17" s="15">
+        <v>0</v>
+      </c>
+      <c r="L17" s="15">
+        <v>0</v>
+      </c>
+      <c r="M17" s="15">
+        <v>0</v>
+      </c>
+      <c r="N17" s="15">
+        <v>0</v>
+      </c>
+      <c r="O17" s="15">
+        <v>1</v>
+      </c>
+      <c r="P17" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="T17" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="J15" s="14" t="s">
+      <c r="U17" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="V17" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="W17" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="X17" s="15"/>
+      <c r="Y17" s="15"/>
+      <c r="Z17" s="15"/>
+      <c r="AA17" s="15"/>
+      <c r="AB17" s="15"/>
+      <c r="AC17" s="15"/>
+      <c r="AD17" s="13"/>
+    </row>
+    <row r="18" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="18"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="16"/>
+      <c r="U18" s="16"/>
+      <c r="V18" s="16"/>
+      <c r="W18" s="16"/>
+      <c r="X18" s="16"/>
+      <c r="Y18" s="16"/>
+      <c r="Z18" s="16"/>
+      <c r="AA18" s="16"/>
+      <c r="AB18" s="16"/>
+      <c r="AC18" s="16"/>
+      <c r="AD18" s="13"/>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="24">
+        <v>1</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="15">
+        <v>0</v>
+      </c>
+      <c r="E19" s="15">
+        <v>0</v>
+      </c>
+      <c r="F19" s="15">
+        <v>0</v>
+      </c>
+      <c r="G19" s="15">
+        <v>1</v>
+      </c>
+      <c r="H19" s="15">
+        <v>0</v>
+      </c>
+      <c r="I19" s="15">
+        <v>110</v>
+      </c>
+      <c r="J19" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="K15" s="14">
-        <v>0</v>
-      </c>
-      <c r="L15" s="14">
-        <v>0</v>
-      </c>
-      <c r="M15" s="14">
-        <v>0</v>
-      </c>
-      <c r="N15" s="14">
-        <v>0</v>
-      </c>
-      <c r="O15" s="14">
-        <v>1</v>
-      </c>
-      <c r="P15" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="T15" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="U15" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="V15" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="W15" s="14" t="s">
+      <c r="K19" s="15">
+        <v>0</v>
+      </c>
+      <c r="L19" s="15">
+        <v>0</v>
+      </c>
+      <c r="M19" s="15">
+        <v>0</v>
+      </c>
+      <c r="N19" s="15">
+        <v>0</v>
+      </c>
+      <c r="O19" s="15">
+        <v>1</v>
+      </c>
+      <c r="P19" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="T19" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="U19" s="15"/>
+      <c r="V19" s="15"/>
+      <c r="W19" s="15"/>
+      <c r="X19" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y19" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="X15" s="14"/>
-      <c r="Y15" s="14"/>
-      <c r="Z15" s="14"/>
-      <c r="AA15" s="14"/>
-      <c r="AB15" s="14"/>
-      <c r="AC15" s="14"/>
-      <c r="AD15" s="35"/>
-    </row>
-    <row r="16" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="34"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="15"/>
-      <c r="Y16" s="15"/>
-      <c r="Z16" s="15"/>
-      <c r="AA16" s="15"/>
-      <c r="AB16" s="15"/>
-      <c r="AC16" s="15"/>
-      <c r="AD16" s="35"/>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A17" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="29">
-        <v>1</v>
-      </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="14">
-        <v>0</v>
-      </c>
-      <c r="E17" s="14">
-        <v>0</v>
-      </c>
-      <c r="F17" s="14">
-        <v>0</v>
-      </c>
-      <c r="G17" s="14">
-        <v>0</v>
-      </c>
-      <c r="H17" s="14">
-        <v>0</v>
-      </c>
-      <c r="I17" s="14">
-        <v>111</v>
-      </c>
-      <c r="J17" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="K17" s="14">
-        <v>0</v>
-      </c>
-      <c r="L17" s="14">
-        <v>0</v>
-      </c>
-      <c r="M17" s="14">
-        <v>0</v>
-      </c>
-      <c r="N17" s="14">
-        <v>0</v>
-      </c>
-      <c r="O17" s="14">
-        <v>1</v>
-      </c>
-      <c r="P17" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="T17" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="U17" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="V17" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="W17" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="X17" s="14"/>
-      <c r="Y17" s="14"/>
-      <c r="Z17" s="14"/>
-      <c r="AA17" s="14"/>
-      <c r="AB17" s="14"/>
-      <c r="AC17" s="14"/>
-      <c r="AD17" s="35"/>
-    </row>
-    <row r="18" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="34"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
-      <c r="S18" s="15"/>
-      <c r="T18" s="15"/>
-      <c r="U18" s="15"/>
-      <c r="V18" s="15"/>
-      <c r="W18" s="15"/>
-      <c r="X18" s="15"/>
-      <c r="Y18" s="15"/>
-      <c r="Z18" s="15"/>
-      <c r="AA18" s="15"/>
-      <c r="AB18" s="15"/>
-      <c r="AC18" s="15"/>
-      <c r="AD18" s="35"/>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A19" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="29">
-        <v>1</v>
-      </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="14">
-        <v>0</v>
-      </c>
-      <c r="E19" s="14">
-        <v>0</v>
-      </c>
-      <c r="F19" s="14">
-        <v>0</v>
-      </c>
-      <c r="G19" s="14">
-        <v>1</v>
-      </c>
-      <c r="H19" s="14">
-        <v>0</v>
-      </c>
-      <c r="I19" s="14">
-        <v>110</v>
-      </c>
-      <c r="J19" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="K19" s="14">
-        <v>0</v>
-      </c>
-      <c r="L19" s="14">
-        <v>0</v>
-      </c>
-      <c r="M19" s="14">
-        <v>0</v>
-      </c>
-      <c r="N19" s="14">
-        <v>0</v>
-      </c>
-      <c r="O19" s="14">
-        <v>1</v>
-      </c>
-      <c r="P19" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="T19" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="U19" s="14"/>
-      <c r="V19" s="14"/>
-      <c r="W19" s="14"/>
-      <c r="X19" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y19" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z19" s="14" t="s">
+      <c r="Z19" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="AA19" s="14"/>
-      <c r="AB19" s="14"/>
-      <c r="AC19" s="14"/>
-      <c r="AD19" s="35"/>
+      <c r="AA19" s="15"/>
+      <c r="AB19" s="15"/>
+      <c r="AC19" s="15"/>
+      <c r="AD19" s="13"/>
     </row>
     <row r="20" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="34"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
-      <c r="T20" s="15"/>
-      <c r="U20" s="15"/>
-      <c r="V20" s="15"/>
-      <c r="W20" s="15"/>
-      <c r="X20" s="15"/>
-      <c r="Y20" s="15"/>
-      <c r="Z20" s="15"/>
-      <c r="AA20" s="15"/>
-      <c r="AB20" s="15"/>
-      <c r="AC20" s="15"/>
-      <c r="AD20" s="35"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="16"/>
+      <c r="V20" s="16"/>
+      <c r="W20" s="16"/>
+      <c r="X20" s="16"/>
+      <c r="Y20" s="16"/>
+      <c r="Z20" s="16"/>
+      <c r="AA20" s="16"/>
+      <c r="AB20" s="16"/>
+      <c r="AC20" s="16"/>
+      <c r="AD20" s="13"/>
     </row>
     <row r="21" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="20">
-        <v>0</v>
-      </c>
-      <c r="C21" s="22"/>
+      <c r="B21" s="19">
+        <v>0</v>
+      </c>
+      <c r="C21" s="20"/>
       <c r="D21" s="2">
         <v>0</v>
       </c>
@@ -2365,7 +2396,7 @@
         <v>23</v>
       </c>
       <c r="T21" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
@@ -2375,19 +2406,19 @@
       </c>
       <c r="Y21" s="4"/>
       <c r="Z21" s="4"/>
-      <c r="AA21" s="9"/>
-      <c r="AB21" s="9"/>
-      <c r="AC21" s="9"/>
-      <c r="AD21" s="35"/>
+      <c r="AA21" s="8"/>
+      <c r="AB21" s="8"/>
+      <c r="AC21" s="8"/>
+      <c r="AD21" s="13"/>
     </row>
     <row r="22" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="20">
-        <v>1</v>
-      </c>
-      <c r="C22" s="22"/>
+      <c r="B22" s="19">
+        <v>1</v>
+      </c>
+      <c r="C22" s="20"/>
       <c r="D22" s="2">
         <v>0</v>
       </c>
@@ -2433,7 +2464,7 @@
         <v>23</v>
       </c>
       <c r="T22" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
@@ -2443,19 +2474,19 @@
         <v>58</v>
       </c>
       <c r="Z22" s="4"/>
-      <c r="AA22" s="9"/>
-      <c r="AB22" s="9"/>
-      <c r="AC22" s="9"/>
-      <c r="AD22" s="35"/>
+      <c r="AA22" s="8"/>
+      <c r="AB22" s="8"/>
+      <c r="AC22" s="8"/>
+      <c r="AD22" s="13"/>
     </row>
     <row r="23" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="20">
-        <v>1</v>
-      </c>
-      <c r="C23" s="22"/>
+      <c r="B23" s="19">
+        <v>1</v>
+      </c>
+      <c r="C23" s="20"/>
       <c r="D23" s="2">
         <v>0</v>
       </c>
@@ -2501,7 +2532,7 @@
         <v>23</v>
       </c>
       <c r="T23" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="U23" s="4"/>
       <c r="V23" s="4"/>
@@ -2513,227 +2544,227 @@
       <c r="Z23" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="AA23" s="9"/>
-      <c r="AB23" s="9"/>
-      <c r="AC23" s="9"/>
-      <c r="AD23" s="35"/>
+      <c r="AA23" s="8"/>
+      <c r="AB23" s="8"/>
+      <c r="AC23" s="8"/>
+      <c r="AD23" s="13"/>
     </row>
     <row r="24" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="29">
-        <v>1</v>
-      </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="14">
-        <v>0</v>
-      </c>
-      <c r="E24" s="14">
-        <v>0</v>
-      </c>
-      <c r="F24" s="14">
-        <v>0</v>
-      </c>
-      <c r="G24" s="14">
-        <v>1</v>
-      </c>
-      <c r="H24" s="14">
-        <v>1</v>
-      </c>
-      <c r="I24" s="14">
+      <c r="B24" s="24">
+        <v>1</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="15">
+        <v>0</v>
+      </c>
+      <c r="E24" s="15">
+        <v>0</v>
+      </c>
+      <c r="F24" s="15">
+        <v>0</v>
+      </c>
+      <c r="G24" s="15">
+        <v>1</v>
+      </c>
+      <c r="H24" s="15">
+        <v>1</v>
+      </c>
+      <c r="I24" s="15">
         <v>110</v>
       </c>
-      <c r="J24" s="14" t="s">
+      <c r="J24" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="K24" s="14">
-        <v>0</v>
-      </c>
-      <c r="L24" s="14">
-        <v>0</v>
-      </c>
-      <c r="M24" s="14">
-        <v>0</v>
-      </c>
-      <c r="N24" s="14">
-        <v>1</v>
-      </c>
-      <c r="O24" s="14">
-        <v>0</v>
-      </c>
-      <c r="P24" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14" t="s">
+      <c r="K24" s="15">
+        <v>0</v>
+      </c>
+      <c r="L24" s="15">
+        <v>0</v>
+      </c>
+      <c r="M24" s="15">
+        <v>0</v>
+      </c>
+      <c r="N24" s="15">
+        <v>1</v>
+      </c>
+      <c r="O24" s="15">
+        <v>0</v>
+      </c>
+      <c r="P24" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="T24" s="14" t="s">
+      <c r="T24" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="U24" s="15"/>
+      <c r="V24" s="15"/>
+      <c r="W24" s="15"/>
+      <c r="X24" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y24" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z24" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA24" s="15"/>
+      <c r="AB24" s="15"/>
+      <c r="AC24" s="15"/>
+      <c r="AD24" s="13"/>
+    </row>
+    <row r="25" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="18"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="16"/>
+      <c r="T25" s="15"/>
+      <c r="U25" s="16"/>
+      <c r="V25" s="16"/>
+      <c r="W25" s="16"/>
+      <c r="X25" s="16"/>
+      <c r="Y25" s="16"/>
+      <c r="Z25" s="16"/>
+      <c r="AA25" s="16"/>
+      <c r="AB25" s="16"/>
+      <c r="AC25" s="16"/>
+      <c r="AD25" s="13"/>
+    </row>
+    <row r="26" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="24">
+        <v>0</v>
+      </c>
+      <c r="C26" s="25"/>
+      <c r="D26" s="15">
+        <v>0</v>
+      </c>
+      <c r="E26" s="15">
+        <v>0</v>
+      </c>
+      <c r="F26" s="15">
+        <v>0</v>
+      </c>
+      <c r="G26" s="15">
+        <v>1</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="15">
+        <v>110</v>
+      </c>
+      <c r="J26" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="K26" s="15">
+        <v>0</v>
+      </c>
+      <c r="L26" s="15">
+        <v>0</v>
+      </c>
+      <c r="M26" s="15">
+        <v>1</v>
+      </c>
+      <c r="N26" s="15">
+        <v>0</v>
+      </c>
+      <c r="O26" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="P26" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="T26" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="U24" s="14"/>
-      <c r="V24" s="14"/>
-      <c r="W24" s="14"/>
-      <c r="X24" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y24" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z24" s="14" t="s">
+      <c r="U26" s="15"/>
+      <c r="V26" s="15"/>
+      <c r="W26" s="15"/>
+      <c r="X26" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y26" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z26" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="AA24" s="14"/>
-      <c r="AB24" s="14"/>
-      <c r="AC24" s="14"/>
-      <c r="AD24" s="35"/>
-    </row>
-    <row r="25" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="34"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
-      <c r="S25" s="15"/>
-      <c r="T25" s="14"/>
-      <c r="U25" s="15"/>
-      <c r="V25" s="15"/>
-      <c r="W25" s="15"/>
-      <c r="X25" s="15"/>
-      <c r="Y25" s="15"/>
-      <c r="Z25" s="15"/>
-      <c r="AA25" s="15"/>
-      <c r="AB25" s="15"/>
-      <c r="AC25" s="15"/>
-      <c r="AD25" s="35"/>
-    </row>
-    <row r="26" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="29">
-        <v>0</v>
-      </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="14">
-        <v>0</v>
-      </c>
-      <c r="E26" s="14">
-        <v>0</v>
-      </c>
-      <c r="F26" s="14">
-        <v>0</v>
-      </c>
-      <c r="G26" s="14">
-        <v>1</v>
-      </c>
-      <c r="H26" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="I26" s="14">
-        <v>110</v>
-      </c>
-      <c r="J26" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="K26" s="14">
-        <v>0</v>
-      </c>
-      <c r="L26" s="14">
-        <v>0</v>
-      </c>
-      <c r="M26" s="14">
-        <v>1</v>
-      </c>
-      <c r="N26" s="14">
-        <v>0</v>
-      </c>
-      <c r="O26" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="P26" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="T26" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="U26" s="14"/>
-      <c r="V26" s="14"/>
-      <c r="W26" s="14"/>
-      <c r="X26" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y26" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z26" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA26" s="14"/>
-      <c r="AB26" s="14"/>
-      <c r="AC26" s="14"/>
-      <c r="AD26" s="35"/>
+      <c r="AA26" s="15"/>
+      <c r="AB26" s="15"/>
+      <c r="AC26" s="15"/>
+      <c r="AD26" s="13"/>
     </row>
     <row r="27" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="34"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="15"/>
-      <c r="T27" s="16"/>
-      <c r="U27" s="15"/>
-      <c r="V27" s="15"/>
-      <c r="W27" s="15"/>
-      <c r="X27" s="15"/>
-      <c r="Y27" s="15"/>
-      <c r="Z27" s="15"/>
-      <c r="AA27" s="15"/>
-      <c r="AB27" s="15"/>
-      <c r="AC27" s="15"/>
-      <c r="AD27" s="35"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="16"/>
+      <c r="T27" s="34"/>
+      <c r="U27" s="16"/>
+      <c r="V27" s="16"/>
+      <c r="W27" s="16"/>
+      <c r="X27" s="16"/>
+      <c r="Y27" s="16"/>
+      <c r="Z27" s="16"/>
+      <c r="AA27" s="16"/>
+      <c r="AB27" s="16"/>
+      <c r="AC27" s="16"/>
+      <c r="AD27" s="13"/>
     </row>
     <row r="28" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="20">
-        <v>0</v>
-      </c>
-      <c r="C28" s="22"/>
+      <c r="B28" s="19">
+        <v>0</v>
+      </c>
+      <c r="C28" s="20"/>
       <c r="D28" s="2">
         <v>0</v>
       </c>
@@ -2779,7 +2810,7 @@
         <v>28</v>
       </c>
       <c r="T28" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U28" s="4"/>
       <c r="V28" s="4"/>
@@ -2787,25 +2818,25 @@
       <c r="X28" s="4"/>
       <c r="Y28" s="4"/>
       <c r="Z28" s="4"/>
-      <c r="AA28" s="9" t="s">
+      <c r="AA28" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AB28" s="9" t="s">
+      <c r="AB28" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AC28" s="9" t="s">
+      <c r="AC28" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="AD28" s="35"/>
+      <c r="AD28" s="13"/>
     </row>
     <row r="29" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="20">
-        <v>0</v>
-      </c>
-      <c r="C29" s="22"/>
+      <c r="B29" s="19">
+        <v>0</v>
+      </c>
+      <c r="C29" s="20"/>
       <c r="D29" s="2">
         <v>0</v>
       </c>
@@ -2857,25 +2888,25 @@
       <c r="X29" s="4"/>
       <c r="Y29" s="4"/>
       <c r="Z29" s="4"/>
-      <c r="AA29" s="9" t="s">
+      <c r="AA29" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AB29" s="9" t="s">
+      <c r="AB29" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AC29" s="9" t="s">
+      <c r="AC29" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="AD29" s="35"/>
+      <c r="AD29" s="13"/>
     </row>
     <row r="30" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="20">
-        <v>0</v>
-      </c>
-      <c r="C30" s="22"/>
+      <c r="B30" s="19">
+        <v>0</v>
+      </c>
+      <c r="C30" s="20"/>
       <c r="D30" s="2">
         <v>0</v>
       </c>
@@ -2921,7 +2952,7 @@
         <v>28</v>
       </c>
       <c r="T30" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U30" s="4"/>
       <c r="V30" s="4"/>
@@ -2929,25 +2960,25 @@
       <c r="X30" s="4"/>
       <c r="Y30" s="4"/>
       <c r="Z30" s="4"/>
-      <c r="AA30" s="9" t="s">
+      <c r="AA30" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AB30" s="9" t="s">
+      <c r="AB30" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AC30" s="9" t="s">
+      <c r="AC30" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="AD30" s="35"/>
+      <c r="AD30" s="13"/>
     </row>
     <row r="31" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="20">
-        <v>0</v>
-      </c>
-      <c r="C31" s="22"/>
+      <c r="B31" s="19">
+        <v>0</v>
+      </c>
+      <c r="C31" s="20"/>
       <c r="D31" s="2">
         <v>0</v>
       </c>
@@ -2993,7 +3024,7 @@
         <v>28</v>
       </c>
       <c r="T31" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="U31" s="4"/>
       <c r="V31" s="4"/>
@@ -3001,25 +3032,25 @@
       <c r="X31" s="4"/>
       <c r="Y31" s="4"/>
       <c r="Z31" s="4"/>
-      <c r="AA31" s="9" t="s">
+      <c r="AA31" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AB31" s="9" t="s">
+      <c r="AB31" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AC31" s="9" t="s">
+      <c r="AC31" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="AD31" s="35"/>
+      <c r="AD31" s="13"/>
     </row>
     <row r="32" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="20">
-        <v>0</v>
-      </c>
-      <c r="C32" s="22"/>
+      <c r="B32" s="19">
+        <v>0</v>
+      </c>
+      <c r="C32" s="20"/>
       <c r="D32" s="2">
         <v>0</v>
       </c>
@@ -3065,7 +3096,7 @@
         <v>28</v>
       </c>
       <c r="T32" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="U32" s="4"/>
       <c r="V32" s="4"/>
@@ -3073,23 +3104,23 @@
       <c r="X32" s="4"/>
       <c r="Y32" s="4"/>
       <c r="Z32" s="4"/>
-      <c r="AA32" s="9" t="s">
+      <c r="AA32" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AB32" s="9" t="s">
+      <c r="AB32" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AC32" s="9" t="s">
+      <c r="AC32" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="AD32" s="35"/>
+      <c r="AD32" s="13"/>
     </row>
     <row r="33" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="22"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="20"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -3115,17 +3146,17 @@
       <c r="X33" s="4"/>
       <c r="Y33" s="4"/>
       <c r="Z33" s="4"/>
-      <c r="AA33" s="9"/>
-      <c r="AB33" s="9"/>
-      <c r="AC33" s="9"/>
-      <c r="AD33" s="35"/>
+      <c r="AA33" s="8"/>
+      <c r="AB33" s="8"/>
+      <c r="AC33" s="8"/>
+      <c r="AD33" s="13"/>
     </row>
     <row r="34" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="22"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="20"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -3151,17 +3182,17 @@
       <c r="X34" s="4"/>
       <c r="Y34" s="4"/>
       <c r="Z34" s="4"/>
-      <c r="AA34" s="9"/>
-      <c r="AB34" s="9"/>
-      <c r="AC34" s="9"/>
-      <c r="AD34" s="35"/>
+      <c r="AA34" s="8"/>
+      <c r="AB34" s="8"/>
+      <c r="AC34" s="8"/>
+      <c r="AD34" s="13"/>
     </row>
     <row r="35" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="20"/>
-      <c r="C35" s="22"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="20"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -3187,17 +3218,17 @@
       <c r="X35" s="4"/>
       <c r="Y35" s="4"/>
       <c r="Z35" s="4"/>
-      <c r="AA35" s="9"/>
-      <c r="AB35" s="9"/>
-      <c r="AC35" s="9"/>
-      <c r="AD35" s="35"/>
+      <c r="AA35" s="8"/>
+      <c r="AB35" s="8"/>
+      <c r="AC35" s="8"/>
+      <c r="AD35" s="13"/>
     </row>
     <row r="36" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="20"/>
-      <c r="C36" s="22"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="20"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -3223,17 +3254,17 @@
       <c r="X36" s="4"/>
       <c r="Y36" s="4"/>
       <c r="Z36" s="4"/>
-      <c r="AA36" s="9"/>
-      <c r="AB36" s="9"/>
-      <c r="AC36" s="9"/>
-      <c r="AD36" s="35"/>
+      <c r="AA36" s="8"/>
+      <c r="AB36" s="8"/>
+      <c r="AC36" s="8"/>
+      <c r="AD36" s="13"/>
     </row>
     <row r="37" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="20"/>
-      <c r="C37" s="22"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="20"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -3259,41 +3290,188 @@
       <c r="X37" s="4"/>
       <c r="Y37" s="4"/>
       <c r="Z37" s="4"/>
-      <c r="AA37" s="9"/>
-      <c r="AB37" s="9"/>
-      <c r="AC37" s="9"/>
-      <c r="AD37" s="35"/>
+      <c r="AA37" s="8"/>
+      <c r="AB37" s="8"/>
+      <c r="AC37" s="8"/>
+      <c r="AD37" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="226">
-    <mergeCell ref="AA19:AA20"/>
-    <mergeCell ref="AB19:AB20"/>
-    <mergeCell ref="AC19:AC20"/>
-    <mergeCell ref="AA24:AA25"/>
-    <mergeCell ref="AB24:AB25"/>
-    <mergeCell ref="AC24:AC25"/>
-    <mergeCell ref="AA26:AA27"/>
-    <mergeCell ref="AB26:AB27"/>
-    <mergeCell ref="AC26:AC27"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="AA13:AA14"/>
-    <mergeCell ref="AB13:AB14"/>
-    <mergeCell ref="AC13:AC14"/>
-    <mergeCell ref="AA15:AA16"/>
-    <mergeCell ref="AB15:AB16"/>
-    <mergeCell ref="AC15:AC16"/>
-    <mergeCell ref="AA17:AA18"/>
-    <mergeCell ref="AB17:AB18"/>
-    <mergeCell ref="AC17:AC18"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
+  <mergeCells count="227">
+    <mergeCell ref="AW1:AX1"/>
+    <mergeCell ref="AM1:AP1"/>
+    <mergeCell ref="AR1:AU1"/>
+    <mergeCell ref="U15:U16"/>
+    <mergeCell ref="V15:V16"/>
+    <mergeCell ref="W15:W16"/>
+    <mergeCell ref="X15:X16"/>
+    <mergeCell ref="Y15:Y16"/>
+    <mergeCell ref="Z15:Z16"/>
+    <mergeCell ref="U17:U18"/>
+    <mergeCell ref="V17:V18"/>
+    <mergeCell ref="W17:W18"/>
+    <mergeCell ref="X17:X18"/>
+    <mergeCell ref="Y17:Y18"/>
+    <mergeCell ref="Z17:Z18"/>
+    <mergeCell ref="X1:Z1"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AS2:AU2"/>
+    <mergeCell ref="AA1:AC1"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="T15:T16"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U19:U20"/>
+    <mergeCell ref="T26:T27"/>
+    <mergeCell ref="T24:T25"/>
+    <mergeCell ref="U24:U25"/>
+    <mergeCell ref="V24:V25"/>
+    <mergeCell ref="W24:W25"/>
+    <mergeCell ref="V19:V20"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="T17:T18"/>
+    <mergeCell ref="T19:T20"/>
+    <mergeCell ref="X24:X25"/>
+    <mergeCell ref="Y24:Y25"/>
+    <mergeCell ref="Z24:Z25"/>
+    <mergeCell ref="U26:U27"/>
+    <mergeCell ref="V26:V27"/>
+    <mergeCell ref="W26:W27"/>
+    <mergeCell ref="X26:X27"/>
+    <mergeCell ref="Y26:Y27"/>
+    <mergeCell ref="Z26:Z27"/>
+    <mergeCell ref="X19:X20"/>
+    <mergeCell ref="Y19:Y20"/>
+    <mergeCell ref="Z19:Z20"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="W13:W14"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="Y13:Y14"/>
+    <mergeCell ref="Z13:Z14"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="B15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="B13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="S15:S16"/>
+    <mergeCell ref="P17:P18"/>
+    <mergeCell ref="Q17:Q18"/>
+    <mergeCell ref="R17:R18"/>
+    <mergeCell ref="S17:S18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="S19:S20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="S24:S25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="B24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="S26:S27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="N26:N27"/>
+    <mergeCell ref="B26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B1:R1"/>
     <mergeCell ref="B28:C28"/>
@@ -3318,180 +3496,34 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="S26:S27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="N26:N27"/>
-    <mergeCell ref="B26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="S24:S25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="S19:S20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="Q19:Q20"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="P17:P18"/>
-    <mergeCell ref="Q17:Q18"/>
-    <mergeCell ref="R17:R18"/>
-    <mergeCell ref="S17:S18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="B15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="B13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="S15:S16"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="X19:X20"/>
-    <mergeCell ref="Y19:Y20"/>
-    <mergeCell ref="Z19:Z20"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="V13:V14"/>
-    <mergeCell ref="W13:W14"/>
-    <mergeCell ref="X13:X14"/>
-    <mergeCell ref="Y13:Y14"/>
-    <mergeCell ref="Z13:Z14"/>
-    <mergeCell ref="X24:X25"/>
-    <mergeCell ref="Y24:Y25"/>
-    <mergeCell ref="Z24:Z25"/>
-    <mergeCell ref="U26:U27"/>
-    <mergeCell ref="V26:V27"/>
-    <mergeCell ref="W26:W27"/>
-    <mergeCell ref="X26:X27"/>
-    <mergeCell ref="Y26:Y27"/>
-    <mergeCell ref="Z26:Z27"/>
-    <mergeCell ref="T15:T16"/>
-    <mergeCell ref="T13:T14"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U19:U20"/>
-    <mergeCell ref="T26:T27"/>
-    <mergeCell ref="T24:T25"/>
-    <mergeCell ref="U24:U25"/>
-    <mergeCell ref="V24:V25"/>
-    <mergeCell ref="W24:W25"/>
-    <mergeCell ref="V19:V20"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="T17:T18"/>
-    <mergeCell ref="T19:T20"/>
-    <mergeCell ref="AM1:AP1"/>
-    <mergeCell ref="AR1:AU1"/>
-    <mergeCell ref="U15:U16"/>
-    <mergeCell ref="V15:V16"/>
-    <mergeCell ref="W15:W16"/>
-    <mergeCell ref="X15:X16"/>
-    <mergeCell ref="Y15:Y16"/>
-    <mergeCell ref="Z15:Z16"/>
-    <mergeCell ref="U17:U18"/>
-    <mergeCell ref="V17:V18"/>
-    <mergeCell ref="W17:W18"/>
-    <mergeCell ref="X17:X18"/>
-    <mergeCell ref="Y17:Y18"/>
-    <mergeCell ref="Z17:Z18"/>
-    <mergeCell ref="X1:Z1"/>
-    <mergeCell ref="U1:W1"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AS2:AU2"/>
-    <mergeCell ref="AA1:AC1"/>
-    <mergeCell ref="AA2:AA3"/>
-    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="AA13:AA14"/>
+    <mergeCell ref="AB13:AB14"/>
+    <mergeCell ref="AC13:AC14"/>
+    <mergeCell ref="AA15:AA16"/>
+    <mergeCell ref="AB15:AB16"/>
+    <mergeCell ref="AC15:AC16"/>
+    <mergeCell ref="AA17:AA18"/>
+    <mergeCell ref="AB17:AB18"/>
+    <mergeCell ref="AC17:AC18"/>
+    <mergeCell ref="AA19:AA20"/>
+    <mergeCell ref="AB19:AB20"/>
+    <mergeCell ref="AC19:AC20"/>
+    <mergeCell ref="AA24:AA25"/>
+    <mergeCell ref="AB24:AB25"/>
+    <mergeCell ref="AC24:AC25"/>
+    <mergeCell ref="AA26:AA27"/>
+    <mergeCell ref="AB26:AB27"/>
+    <mergeCell ref="AC26:AC27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding Flush for ret and fixing some issues
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\CCE\Year 3 - Senior 1\Semester 2\Arch\Project\Repo\Architecture-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8712638E-325D-4643-AD93-E5C5E80C38E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3A4837-0117-49C5-BB62-A693435C13C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="390" windowWidth="25440" windowHeight="15390" xr2:uid="{0E858663-1FD8-418A-96F6-784D0D9CF43C}"/>
   </bookViews>
@@ -661,12 +661,57 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -679,53 +724,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1043,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9834DC43-CD6B-4773-9F5D-9D470392FD57}">
   <dimension ref="A1:AX37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AE22" sqref="AE22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1085,46 +1085,46 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
+      <c r="B1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
       <c r="S1" s="14" t="s">
         <v>2</v>
       </c>
       <c r="T1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="U1" s="23" t="s">
+      <c r="U1" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="V1" s="24"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="23" t="s">
+      <c r="V1" s="28"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="23" t="s">
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
       <c r="AD1" s="13"/>
       <c r="AE1" s="14" t="s">
         <v>37</v>
@@ -1132,28 +1132,28 @@
       <c r="AF1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="AH1" s="26" t="s">
+      <c r="AH1" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="28"/>
-      <c r="AM1" s="26" t="s">
+      <c r="AI1" s="42"/>
+      <c r="AJ1" s="42"/>
+      <c r="AK1" s="43"/>
+      <c r="AM1" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="28"/>
-      <c r="AR1" s="26" t="s">
+      <c r="AN1" s="42"/>
+      <c r="AO1" s="42"/>
+      <c r="AP1" s="43"/>
+      <c r="AR1" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="28"/>
-      <c r="AW1" s="26" t="s">
+      <c r="AS1" s="42"/>
+      <c r="AT1" s="42"/>
+      <c r="AU1" s="43"/>
+      <c r="AW1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="AX1" s="27"/>
+      <c r="AX1" s="42"/>
     </row>
     <row r="2" spans="1:50" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
@@ -1275,11 +1275,11 @@
       <c r="AR2" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="AS2" s="29" t="s">
+      <c r="AS2" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="AT2" s="30"/>
-      <c r="AU2" s="31"/>
+      <c r="AT2" s="44"/>
+      <c r="AU2" s="26"/>
       <c r="AV2" s="16"/>
       <c r="AW2" s="9" t="s">
         <v>102</v>
@@ -1330,10 +1330,10 @@
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="29">
-        <v>0</v>
-      </c>
-      <c r="C4" s="31"/>
+      <c r="B4" s="25">
+        <v>0</v>
+      </c>
+      <c r="C4" s="26"/>
       <c r="D4" s="2">
         <v>0</v>
       </c>
@@ -1402,10 +1402,10 @@
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="29">
-        <v>0</v>
-      </c>
-      <c r="C5" s="31"/>
+      <c r="B5" s="25">
+        <v>0</v>
+      </c>
+      <c r="C5" s="26"/>
       <c r="D5" s="2">
         <v>0</v>
       </c>
@@ -1474,10 +1474,10 @@
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="29">
-        <v>0</v>
-      </c>
-      <c r="C6" s="31"/>
+      <c r="B6" s="25">
+        <v>0</v>
+      </c>
+      <c r="C6" s="26"/>
       <c r="D6" s="2">
         <v>0</v>
       </c>
@@ -1556,10 +1556,10 @@
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="29">
-        <v>1</v>
-      </c>
-      <c r="C7" s="31"/>
+      <c r="B7" s="25">
+        <v>1</v>
+      </c>
+      <c r="C7" s="26"/>
       <c r="D7" s="2">
         <v>0</v>
       </c>
@@ -1638,10 +1638,10 @@
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="29">
-        <v>1</v>
-      </c>
-      <c r="C8" s="31"/>
+      <c r="B8" s="25">
+        <v>1</v>
+      </c>
+      <c r="C8" s="26"/>
       <c r="D8" s="2">
         <v>0</v>
       </c>
@@ -1720,10 +1720,10 @@
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="29">
-        <v>0</v>
-      </c>
-      <c r="C9" s="31"/>
+      <c r="B9" s="25">
+        <v>0</v>
+      </c>
+      <c r="C9" s="26"/>
       <c r="D9" s="2">
         <v>0</v>
       </c>
@@ -1802,10 +1802,10 @@
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="29">
-        <v>1</v>
-      </c>
-      <c r="C10" s="31"/>
+      <c r="B10" s="25">
+        <v>1</v>
+      </c>
+      <c r="C10" s="26"/>
       <c r="D10" s="2">
         <v>1</v>
       </c>
@@ -1884,10 +1884,10 @@
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="29">
-        <v>1</v>
-      </c>
-      <c r="C11" s="31"/>
+      <c r="B11" s="25">
+        <v>1</v>
+      </c>
+      <c r="C11" s="26"/>
       <c r="D11" s="2">
         <v>0</v>
       </c>
@@ -1966,10 +1966,10 @@
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="29">
-        <v>1</v>
-      </c>
-      <c r="C12" s="31"/>
+      <c r="B12" s="25">
+        <v>1</v>
+      </c>
+      <c r="C12" s="26"/>
       <c r="D12" s="2">
         <v>0</v>
       </c>
@@ -2039,13 +2039,13 @@
       <c r="AD12" s="12"/>
     </row>
     <row r="13" spans="1:50" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="39">
-        <v>1</v>
-      </c>
-      <c r="C13" s="40"/>
+      <c r="B13" s="29">
+        <v>1</v>
+      </c>
+      <c r="C13" s="30"/>
       <c r="D13" s="21">
         <v>0</v>
       </c>
@@ -2121,9 +2121,9 @@
       </c>
     </row>
     <row r="14" spans="1:50" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="44"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="42"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="32"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
@@ -2159,13 +2159,13 @@
       </c>
     </row>
     <row r="15" spans="1:50" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="39">
-        <v>1</v>
-      </c>
-      <c r="C15" s="40"/>
+      <c r="B15" s="29">
+        <v>1</v>
+      </c>
+      <c r="C15" s="30"/>
       <c r="D15" s="21">
         <v>0</v>
       </c>
@@ -2241,9 +2241,9 @@
       </c>
     </row>
     <row r="16" spans="1:50" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="44"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="42"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="32"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
@@ -2277,13 +2277,13 @@
       <c r="AF16" s="18"/>
     </row>
     <row r="17" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="39">
-        <v>1</v>
-      </c>
-      <c r="C17" s="40"/>
+      <c r="B17" s="29">
+        <v>1</v>
+      </c>
+      <c r="C17" s="30"/>
       <c r="D17" s="21">
         <v>0</v>
       </c>
@@ -2357,9 +2357,9 @@
       <c r="AF17" s="18"/>
     </row>
     <row r="18" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="44"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="42"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
@@ -2389,13 +2389,13 @@
       <c r="AD18" s="12"/>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="39">
-        <v>1</v>
-      </c>
-      <c r="C19" s="40"/>
+      <c r="B19" s="29">
+        <v>1</v>
+      </c>
+      <c r="C19" s="30"/>
       <c r="D19" s="21">
         <v>0</v>
       </c>
@@ -2465,9 +2465,9 @@
       <c r="AD19" s="12"/>
     </row>
     <row r="20" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="44"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="42"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="32"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
@@ -2500,10 +2500,10 @@
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="29">
-        <v>0</v>
-      </c>
-      <c r="C21" s="31"/>
+      <c r="B21" s="25">
+        <v>0</v>
+      </c>
+      <c r="C21" s="26"/>
       <c r="D21" s="2">
         <v>0</v>
       </c>
@@ -2572,10 +2572,10 @@
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="29">
-        <v>1</v>
-      </c>
-      <c r="C22" s="31"/>
+      <c r="B22" s="25">
+        <v>1</v>
+      </c>
+      <c r="C22" s="26"/>
       <c r="D22" s="2">
         <v>0</v>
       </c>
@@ -2644,10 +2644,10 @@
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="29">
-        <v>1</v>
-      </c>
-      <c r="C23" s="31"/>
+      <c r="B23" s="25">
+        <v>1</v>
+      </c>
+      <c r="C23" s="26"/>
       <c r="D23" s="2">
         <v>0</v>
       </c>
@@ -2715,13 +2715,13 @@
       <c r="AD23" s="12"/>
     </row>
     <row r="24" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="39">
-        <v>1</v>
-      </c>
-      <c r="C24" s="40"/>
+      <c r="B24" s="29">
+        <v>1</v>
+      </c>
+      <c r="C24" s="30"/>
       <c r="D24" s="21">
         <v>0</v>
       </c>
@@ -2791,9 +2791,9 @@
       <c r="AD24" s="12"/>
     </row>
     <row r="25" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="44"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="42"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="32"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
@@ -2823,13 +2823,13 @@
       <c r="AD25" s="12"/>
     </row>
     <row r="26" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="43" t="s">
+      <c r="A26" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="39">
-        <v>0</v>
-      </c>
-      <c r="C26" s="40"/>
+      <c r="B26" s="29">
+        <v>0</v>
+      </c>
+      <c r="C26" s="30"/>
       <c r="D26" s="21">
         <v>0</v>
       </c>
@@ -2899,9 +2899,9 @@
       <c r="AD26" s="12"/>
     </row>
     <row r="27" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="44"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="42"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="32"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
@@ -2918,7 +2918,7 @@
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="22"/>
-      <c r="T27" s="32"/>
+      <c r="T27" s="39"/>
       <c r="U27" s="22"/>
       <c r="V27" s="22"/>
       <c r="W27" s="22"/>
@@ -2934,10 +2934,10 @@
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="29">
-        <v>0</v>
-      </c>
-      <c r="C28" s="31"/>
+      <c r="B28" s="25">
+        <v>0</v>
+      </c>
+      <c r="C28" s="26"/>
       <c r="D28" s="2">
         <v>0</v>
       </c>
@@ -3010,10 +3010,10 @@
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="29">
-        <v>0</v>
-      </c>
-      <c r="C29" s="31"/>
+      <c r="B29" s="25">
+        <v>0</v>
+      </c>
+      <c r="C29" s="26"/>
       <c r="D29" s="2">
         <v>0</v>
       </c>
@@ -3084,10 +3084,10 @@
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="29">
-        <v>0</v>
-      </c>
-      <c r="C30" s="31"/>
+      <c r="B30" s="25">
+        <v>0</v>
+      </c>
+      <c r="C30" s="26"/>
       <c r="D30" s="2">
         <v>0</v>
       </c>
@@ -3160,10 +3160,10 @@
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="29">
-        <v>0</v>
-      </c>
-      <c r="C31" s="31"/>
+      <c r="B31" s="25">
+        <v>0</v>
+      </c>
+      <c r="C31" s="26"/>
       <c r="D31" s="2">
         <v>0</v>
       </c>
@@ -3236,10 +3236,10 @@
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="29">
-        <v>0</v>
-      </c>
-      <c r="C32" s="31"/>
+      <c r="B32" s="25">
+        <v>0</v>
+      </c>
+      <c r="C32" s="26"/>
       <c r="D32" s="2">
         <v>0</v>
       </c>
@@ -3312,10 +3312,10 @@
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="29">
-        <v>0</v>
-      </c>
-      <c r="C33" s="31"/>
+      <c r="B33" s="25">
+        <v>0</v>
+      </c>
+      <c r="C33" s="26"/>
       <c r="D33" s="2">
         <v>0</v>
       </c>
@@ -3360,10 +3360,10 @@
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="29">
-        <v>0</v>
-      </c>
-      <c r="C34" s="31"/>
+      <c r="B34" s="25">
+        <v>0</v>
+      </c>
+      <c r="C34" s="26"/>
       <c r="D34" s="2">
         <v>0</v>
       </c>
@@ -3408,10 +3408,10 @@
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="29">
-        <v>0</v>
-      </c>
-      <c r="C35" s="31"/>
+      <c r="B35" s="25">
+        <v>0</v>
+      </c>
+      <c r="C35" s="26"/>
       <c r="D35" s="2">
         <v>0</v>
       </c>
@@ -3456,8 +3456,8 @@
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="29"/>
-      <c r="C36" s="31"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="26"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -3492,8 +3492,8 @@
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="29"/>
-      <c r="C37" s="31"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="26"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -3526,119 +3526,96 @@
     </row>
   </sheetData>
   <mergeCells count="227">
-    <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="R15:R16"/>
-    <mergeCell ref="R17:R18"/>
-    <mergeCell ref="R19:R20"/>
-    <mergeCell ref="Q15:Q16"/>
-    <mergeCell ref="Q17:Q18"/>
-    <mergeCell ref="Q19:Q20"/>
-    <mergeCell ref="Q24:Q25"/>
-    <mergeCell ref="R24:R25"/>
-    <mergeCell ref="AA26:AA27"/>
-    <mergeCell ref="AB26:AB27"/>
-    <mergeCell ref="AC26:AC27"/>
-    <mergeCell ref="AA17:AA18"/>
-    <mergeCell ref="AB17:AB18"/>
-    <mergeCell ref="AC17:AC18"/>
-    <mergeCell ref="AA19:AA20"/>
-    <mergeCell ref="AB19:AB20"/>
-    <mergeCell ref="AC19:AC20"/>
-    <mergeCell ref="AA24:AA25"/>
-    <mergeCell ref="AB24:AB25"/>
-    <mergeCell ref="AC24:AC25"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B1:R1"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="N26:N27"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="P26:P27"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="P24:P25"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="P15:P16"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="S26:S27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="B26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="Q26:Q27"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="S24:S25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="S19:S20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="P17:P18"/>
-    <mergeCell ref="S17:S18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="AB15:AB16"/>
+    <mergeCell ref="AC15:AC16"/>
+    <mergeCell ref="X1:Z1"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="AW1:AX1"/>
+    <mergeCell ref="AM1:AP1"/>
+    <mergeCell ref="AR1:AU1"/>
+    <mergeCell ref="U15:U16"/>
+    <mergeCell ref="V15:V16"/>
+    <mergeCell ref="W15:W16"/>
+    <mergeCell ref="X15:X16"/>
+    <mergeCell ref="Y15:Y16"/>
+    <mergeCell ref="Z15:Z16"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AS2:AU2"/>
+    <mergeCell ref="AA1:AC1"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="AA13:AA14"/>
+    <mergeCell ref="AB13:AB14"/>
+    <mergeCell ref="AC13:AC14"/>
+    <mergeCell ref="AA15:AA16"/>
+    <mergeCell ref="T15:T16"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U19:U20"/>
+    <mergeCell ref="T26:T27"/>
+    <mergeCell ref="T24:T25"/>
+    <mergeCell ref="U24:U25"/>
+    <mergeCell ref="V24:V25"/>
+    <mergeCell ref="W24:W25"/>
+    <mergeCell ref="V19:V20"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="T17:T18"/>
+    <mergeCell ref="T19:T20"/>
+    <mergeCell ref="U17:U18"/>
+    <mergeCell ref="V17:V18"/>
+    <mergeCell ref="W17:W18"/>
+    <mergeCell ref="X24:X25"/>
+    <mergeCell ref="Y24:Y25"/>
+    <mergeCell ref="Z24:Z25"/>
+    <mergeCell ref="U26:U27"/>
+    <mergeCell ref="V26:V27"/>
+    <mergeCell ref="W26:W27"/>
+    <mergeCell ref="X26:X27"/>
+    <mergeCell ref="Y26:Y27"/>
+    <mergeCell ref="Z26:Z27"/>
+    <mergeCell ref="X19:X20"/>
+    <mergeCell ref="Y19:Y20"/>
+    <mergeCell ref="Z19:Z20"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="W13:W14"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="Y13:Y14"/>
+    <mergeCell ref="Z13:Z14"/>
+    <mergeCell ref="X17:X18"/>
+    <mergeCell ref="Y17:Y18"/>
+    <mergeCell ref="Z17:Z18"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
     <mergeCell ref="S13:S14"/>
     <mergeCell ref="B15:C16"/>
     <mergeCell ref="D15:D16"/>
@@ -3663,96 +3640,119 @@
     <mergeCell ref="S15:S16"/>
     <mergeCell ref="M15:M16"/>
     <mergeCell ref="N15:N16"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="V13:V14"/>
-    <mergeCell ref="W13:W14"/>
-    <mergeCell ref="X13:X14"/>
-    <mergeCell ref="Y13:Y14"/>
-    <mergeCell ref="Z13:Z14"/>
-    <mergeCell ref="X17:X18"/>
-    <mergeCell ref="Y17:Y18"/>
-    <mergeCell ref="Z17:Z18"/>
-    <mergeCell ref="U26:U27"/>
-    <mergeCell ref="V26:V27"/>
-    <mergeCell ref="W26:W27"/>
-    <mergeCell ref="X26:X27"/>
-    <mergeCell ref="Y26:Y27"/>
-    <mergeCell ref="Z26:Z27"/>
-    <mergeCell ref="X19:X20"/>
-    <mergeCell ref="Y19:Y20"/>
-    <mergeCell ref="Z19:Z20"/>
-    <mergeCell ref="AC13:AC14"/>
-    <mergeCell ref="AA15:AA16"/>
-    <mergeCell ref="T15:T16"/>
-    <mergeCell ref="T13:T14"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U19:U20"/>
-    <mergeCell ref="T26:T27"/>
-    <mergeCell ref="T24:T25"/>
-    <mergeCell ref="U24:U25"/>
-    <mergeCell ref="V24:V25"/>
-    <mergeCell ref="W24:W25"/>
-    <mergeCell ref="V19:V20"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="T17:T18"/>
-    <mergeCell ref="T19:T20"/>
-    <mergeCell ref="U17:U18"/>
-    <mergeCell ref="V17:V18"/>
-    <mergeCell ref="W17:W18"/>
-    <mergeCell ref="X24:X25"/>
-    <mergeCell ref="Y24:Y25"/>
-    <mergeCell ref="Z24:Z25"/>
-    <mergeCell ref="AB15:AB16"/>
-    <mergeCell ref="AC15:AC16"/>
-    <mergeCell ref="X1:Z1"/>
-    <mergeCell ref="U1:W1"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="AW1:AX1"/>
-    <mergeCell ref="AM1:AP1"/>
-    <mergeCell ref="AR1:AU1"/>
-    <mergeCell ref="U15:U16"/>
-    <mergeCell ref="V15:V16"/>
-    <mergeCell ref="W15:W16"/>
-    <mergeCell ref="X15:X16"/>
-    <mergeCell ref="Y15:Y16"/>
-    <mergeCell ref="Z15:Z16"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AS2:AU2"/>
-    <mergeCell ref="AA1:AC1"/>
-    <mergeCell ref="AA2:AA3"/>
-    <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="AA13:AA14"/>
-    <mergeCell ref="AB13:AB14"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="P17:P18"/>
+    <mergeCell ref="S17:S18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="S19:S20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="S24:S25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="B24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="S26:S27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="B26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="Q26:Q27"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B1:R1"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="N26:N27"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="P26:P27"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="P24:P25"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="P15:P16"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="AA26:AA27"/>
+    <mergeCell ref="AB26:AB27"/>
+    <mergeCell ref="AC26:AC27"/>
+    <mergeCell ref="AA17:AA18"/>
+    <mergeCell ref="AB17:AB18"/>
+    <mergeCell ref="AC17:AC18"/>
+    <mergeCell ref="AA19:AA20"/>
+    <mergeCell ref="AB19:AB20"/>
+    <mergeCell ref="AC19:AC20"/>
+    <mergeCell ref="AA24:AA25"/>
+    <mergeCell ref="AB24:AB25"/>
+    <mergeCell ref="AC24:AC25"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="R15:R16"/>
+    <mergeCell ref="R17:R18"/>
+    <mergeCell ref="R19:R20"/>
+    <mergeCell ref="Q15:Q16"/>
+    <mergeCell ref="Q17:Q18"/>
+    <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="Q24:Q25"/>
+    <mergeCell ref="R24:R25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding Files for the components required in the Execution Stage
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\CCE\Year 3 - Senior 1\Semester 2\Arch\Project\Repo\Architecture-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD3266A-883D-4739-B1B5-C4E5EB3186E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B09EECB-E24F-4A7C-BFB0-28F191512978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="390" windowWidth="25440" windowHeight="15390" xr2:uid="{0E858663-1FD8-418A-96F6-784D0D9CF43C}"/>
   </bookViews>
@@ -725,68 +725,68 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1104,7 +1104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9834DC43-CD6B-4773-9F5D-9D470392FD57}">
   <dimension ref="A1:BA40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AJ22" sqref="AJ22"/>
     </sheetView>
   </sheetViews>
@@ -1146,25 +1146,25 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
+      <c r="B1" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
       <c r="S1" s="22"/>
       <c r="T1" s="22"/>
       <c r="U1" s="22"/>
@@ -1174,21 +1174,21 @@
       <c r="W1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="X1" s="39" t="s">
+      <c r="X1" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="Y1" s="40"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="39" t="s">
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="AB1" s="40"/>
-      <c r="AC1" s="40"/>
-      <c r="AD1" s="39" t="s">
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="AE1" s="40"/>
-      <c r="AF1" s="40"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
       <c r="AG1" s="13"/>
       <c r="AH1" s="14" t="s">
         <v>37</v>
@@ -1196,71 +1196,71 @@
       <c r="AI1" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="AK1" s="48" t="s">
+      <c r="AK1" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="AL1" s="49"/>
-      <c r="AM1" s="49"/>
-      <c r="AN1" s="50"/>
-      <c r="AP1" s="48" t="s">
+      <c r="AL1" s="35"/>
+      <c r="AM1" s="35"/>
+      <c r="AN1" s="36"/>
+      <c r="AP1" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="AQ1" s="49"/>
-      <c r="AR1" s="49"/>
-      <c r="AS1" s="50"/>
-      <c r="AU1" s="48" t="s">
+      <c r="AQ1" s="35"/>
+      <c r="AR1" s="35"/>
+      <c r="AS1" s="36"/>
+      <c r="AU1" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="AV1" s="49"/>
-      <c r="AW1" s="49"/>
-      <c r="AX1" s="50"/>
-      <c r="AZ1" s="48" t="s">
+      <c r="AV1" s="35"/>
+      <c r="AW1" s="35"/>
+      <c r="AX1" s="36"/>
+      <c r="AZ1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="BA1" s="49"/>
+      <c r="BA1" s="35"/>
     </row>
     <row r="2" spans="1:53" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="41" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="F2" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="I2" s="41" t="s">
+      <c r="I2" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="41" t="s">
+      <c r="J2" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="41" t="s">
+      <c r="K2" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="41" t="s">
+      <c r="L2" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="41" t="s">
+      <c r="M2" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="N2" s="41" t="s">
+      <c r="N2" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="O2" s="41" t="s">
+      <c r="O2" s="40" t="s">
         <v>11</v>
       </c>
       <c r="P2" s="29" t="s">
@@ -1348,11 +1348,11 @@
       <c r="AU2" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="AV2" s="33" t="s">
+      <c r="AV2" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="AW2" s="51"/>
-      <c r="AX2" s="34"/>
+      <c r="AW2" s="38"/>
+      <c r="AX2" s="39"/>
       <c r="AY2" s="16"/>
       <c r="AZ2" s="9" t="s">
         <v>98</v>
@@ -1363,20 +1363,20 @@
     </row>
     <row r="3" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="30"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="42"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
       <c r="P3" s="30"/>
       <c r="Q3" s="30"/>
       <c r="R3" s="30"/>
@@ -1406,10 +1406,10 @@
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="33">
-        <v>0</v>
-      </c>
-      <c r="C4" s="34"/>
+      <c r="B4" s="37">
+        <v>0</v>
+      </c>
+      <c r="C4" s="39"/>
       <c r="D4" s="2">
         <v>0</v>
       </c>
@@ -1489,10 +1489,10 @@
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="33">
-        <v>0</v>
-      </c>
-      <c r="C5" s="34"/>
+      <c r="B5" s="37">
+        <v>0</v>
+      </c>
+      <c r="C5" s="39"/>
       <c r="D5" s="2">
         <v>0</v>
       </c>
@@ -1572,10 +1572,10 @@
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="33">
-        <v>0</v>
-      </c>
-      <c r="C6" s="34"/>
+      <c r="B6" s="37">
+        <v>0</v>
+      </c>
+      <c r="C6" s="39"/>
       <c r="D6" s="2">
         <v>0</v>
       </c>
@@ -1663,10 +1663,10 @@
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="33">
-        <v>1</v>
-      </c>
-      <c r="C7" s="34"/>
+      <c r="B7" s="37">
+        <v>1</v>
+      </c>
+      <c r="C7" s="39"/>
       <c r="D7" s="2">
         <v>0</v>
       </c>
@@ -1754,10 +1754,10 @@
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="33">
-        <v>1</v>
-      </c>
-      <c r="C8" s="34"/>
+      <c r="B8" s="37">
+        <v>1</v>
+      </c>
+      <c r="C8" s="39"/>
       <c r="D8" s="2">
         <v>0</v>
       </c>
@@ -1845,10 +1845,10 @@
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="33">
-        <v>0</v>
-      </c>
-      <c r="C9" s="34"/>
+      <c r="B9" s="37">
+        <v>0</v>
+      </c>
+      <c r="C9" s="39"/>
       <c r="D9" s="2">
         <v>0</v>
       </c>
@@ -1936,10 +1936,10 @@
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="33">
-        <v>1</v>
-      </c>
-      <c r="C10" s="34"/>
+      <c r="B10" s="37">
+        <v>1</v>
+      </c>
+      <c r="C10" s="39"/>
       <c r="D10" s="2">
         <v>1</v>
       </c>
@@ -2027,10 +2027,10 @@
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="33">
-        <v>1</v>
-      </c>
-      <c r="C11" s="34"/>
+      <c r="B11" s="37">
+        <v>1</v>
+      </c>
+      <c r="C11" s="39"/>
       <c r="D11" s="2">
         <v>0</v>
       </c>
@@ -2118,10 +2118,10 @@
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="33">
-        <v>1</v>
-      </c>
-      <c r="C12" s="34"/>
+      <c r="B12" s="37">
+        <v>1</v>
+      </c>
+      <c r="C12" s="39"/>
       <c r="D12" s="2">
         <v>0</v>
       </c>
@@ -2206,13 +2206,13 @@
       </c>
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="35">
-        <v>1</v>
-      </c>
-      <c r="C13" s="36"/>
+      <c r="B13" s="46">
+        <v>1</v>
+      </c>
+      <c r="C13" s="47"/>
       <c r="D13" s="29">
         <v>0</v>
       </c>
@@ -2291,9 +2291,9 @@
       <c r="AG13" s="12"/>
     </row>
     <row r="14" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="32"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="38"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="49"/>
       <c r="D14" s="30"/>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
@@ -2326,13 +2326,13 @@
       <c r="AG14" s="12"/>
     </row>
     <row r="15" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="35">
-        <v>1</v>
-      </c>
-      <c r="C15" s="36"/>
+      <c r="B15" s="46">
+        <v>1</v>
+      </c>
+      <c r="C15" s="47"/>
       <c r="D15" s="29">
         <v>0</v>
       </c>
@@ -2411,9 +2411,9 @@
       <c r="AG15" s="12"/>
     </row>
     <row r="16" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="32"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="38"/>
+      <c r="A16" s="51"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="49"/>
       <c r="D16" s="30"/>
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
@@ -2449,13 +2449,13 @@
       <c r="AK16" s="28"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="35">
-        <v>1</v>
-      </c>
-      <c r="C17" s="36"/>
+      <c r="B17" s="46">
+        <v>1</v>
+      </c>
+      <c r="C17" s="47"/>
       <c r="D17" s="29">
         <v>0</v>
       </c>
@@ -2534,9 +2534,9 @@
       <c r="AG17" s="12"/>
     </row>
     <row r="18" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="32"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="38"/>
+      <c r="A18" s="51"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="49"/>
       <c r="D18" s="30"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
@@ -2569,13 +2569,13 @@
       <c r="AG18" s="12"/>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="35">
-        <v>1</v>
-      </c>
-      <c r="C19" s="36"/>
+      <c r="B19" s="46">
+        <v>1</v>
+      </c>
+      <c r="C19" s="47"/>
       <c r="D19" s="29">
         <v>0</v>
       </c>
@@ -2654,9 +2654,9 @@
       <c r="AG19" s="12"/>
     </row>
     <row r="20" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="32"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="38"/>
+      <c r="A20" s="51"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="49"/>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
       <c r="F20" s="30"/>
@@ -2692,10 +2692,10 @@
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="33">
-        <v>0</v>
-      </c>
-      <c r="C21" s="34"/>
+      <c r="B21" s="37">
+        <v>0</v>
+      </c>
+      <c r="C21" s="39"/>
       <c r="D21" s="2">
         <v>0</v>
       </c>
@@ -2773,10 +2773,10 @@
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="33">
-        <v>1</v>
-      </c>
-      <c r="C22" s="34"/>
+      <c r="B22" s="37">
+        <v>1</v>
+      </c>
+      <c r="C22" s="39"/>
       <c r="D22" s="2">
         <v>0</v>
       </c>
@@ -2860,10 +2860,10 @@
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="33">
-        <v>1</v>
-      </c>
-      <c r="C23" s="34"/>
+      <c r="B23" s="37">
+        <v>1</v>
+      </c>
+      <c r="C23" s="39"/>
       <c r="D23" s="2">
         <v>0</v>
       </c>
@@ -2945,14 +2945,14 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:35" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="31" t="s">
+    <row r="24" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="35">
-        <v>1</v>
-      </c>
-      <c r="C24" s="36"/>
+      <c r="B24" s="46">
+        <v>1</v>
+      </c>
+      <c r="C24" s="47"/>
       <c r="D24" s="29">
         <v>0</v>
       </c>
@@ -3037,9 +3037,9 @@
       </c>
     </row>
     <row r="25" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="32"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="38"/>
+      <c r="A25" s="51"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="49"/>
       <c r="D25" s="30"/>
       <c r="E25" s="30"/>
       <c r="F25" s="30"/>
@@ -3078,13 +3078,13 @@
       </c>
     </row>
     <row r="26" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="35">
-        <v>0</v>
-      </c>
-      <c r="C26" s="36"/>
+      <c r="B26" s="46">
+        <v>0</v>
+      </c>
+      <c r="C26" s="47"/>
       <c r="D26" s="29">
         <v>0</v>
       </c>
@@ -3169,9 +3169,9 @@
       </c>
     </row>
     <row r="27" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="32"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="38"/>
+      <c r="A27" s="51"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="49"/>
       <c r="D27" s="30"/>
       <c r="E27" s="30"/>
       <c r="F27" s="30"/>
@@ -3207,10 +3207,10 @@
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="33">
-        <v>0</v>
-      </c>
-      <c r="C28" s="34"/>
+      <c r="B28" s="37">
+        <v>0</v>
+      </c>
+      <c r="C28" s="39"/>
       <c r="D28" s="2">
         <v>0</v>
       </c>
@@ -3292,10 +3292,10 @@
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="33">
-        <v>0</v>
-      </c>
-      <c r="C29" s="34"/>
+      <c r="B29" s="37">
+        <v>0</v>
+      </c>
+      <c r="C29" s="39"/>
       <c r="D29" s="2">
         <v>0</v>
       </c>
@@ -3377,10 +3377,10 @@
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="33">
-        <v>0</v>
-      </c>
-      <c r="C30" s="34"/>
+      <c r="B30" s="37">
+        <v>0</v>
+      </c>
+      <c r="C30" s="39"/>
       <c r="D30" s="2">
         <v>0</v>
       </c>
@@ -3462,10 +3462,10 @@
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="33">
-        <v>0</v>
-      </c>
-      <c r="C31" s="34"/>
+      <c r="B31" s="37">
+        <v>0</v>
+      </c>
+      <c r="C31" s="39"/>
       <c r="D31" s="2">
         <v>0</v>
       </c>
@@ -3547,10 +3547,10 @@
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="33">
-        <v>0</v>
-      </c>
-      <c r="C32" s="34"/>
+      <c r="B32" s="37">
+        <v>0</v>
+      </c>
+      <c r="C32" s="39"/>
       <c r="D32" s="2">
         <v>0</v>
       </c>
@@ -3632,10 +3632,10 @@
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="33">
-        <v>0</v>
-      </c>
-      <c r="C33" s="34"/>
+      <c r="B33" s="37">
+        <v>0</v>
+      </c>
+      <c r="C33" s="39"/>
       <c r="D33" s="2">
         <v>0</v>
       </c>
@@ -3717,10 +3717,10 @@
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="33">
-        <v>0</v>
-      </c>
-      <c r="C34" s="34"/>
+      <c r="B34" s="37">
+        <v>0</v>
+      </c>
+      <c r="C34" s="39"/>
       <c r="D34" s="2">
         <v>0</v>
       </c>
@@ -3802,10 +3802,10 @@
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="33">
-        <v>0</v>
-      </c>
-      <c r="C35" s="34"/>
+      <c r="B35" s="37">
+        <v>0</v>
+      </c>
+      <c r="C35" s="39"/>
       <c r="D35" s="2">
         <v>0</v>
       </c>
@@ -3894,8 +3894,8 @@
       <c r="A39" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="33"/>
-      <c r="C39" s="34"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="39"/>
       <c r="D39" s="21"/>
       <c r="E39" s="21"/>
       <c r="F39" s="21"/>
@@ -3930,8 +3930,8 @@
       <c r="A40" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="33"/>
-      <c r="C40" s="34"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="39"/>
       <c r="D40" s="23"/>
       <c r="E40" s="23"/>
       <c r="F40" s="23"/>
@@ -3964,6 +3964,230 @@
     </row>
   </sheetData>
   <mergeCells count="248">
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="U15:U16"/>
+    <mergeCell ref="U17:U18"/>
+    <mergeCell ref="U19:U20"/>
+    <mergeCell ref="U24:U25"/>
+    <mergeCell ref="U26:U27"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="S15:S16"/>
+    <mergeCell ref="S17:S18"/>
+    <mergeCell ref="S19:S20"/>
+    <mergeCell ref="S24:S25"/>
+    <mergeCell ref="S26:S27"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="T15:T16"/>
+    <mergeCell ref="T17:T18"/>
+    <mergeCell ref="T19:T20"/>
+    <mergeCell ref="T24:T25"/>
+    <mergeCell ref="T26:T27"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="R15:R16"/>
+    <mergeCell ref="R17:R18"/>
+    <mergeCell ref="R19:R20"/>
+    <mergeCell ref="Q15:Q16"/>
+    <mergeCell ref="Q17:Q18"/>
+    <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="Q24:Q25"/>
+    <mergeCell ref="R24:R25"/>
+    <mergeCell ref="AD26:AD27"/>
+    <mergeCell ref="AE26:AE27"/>
+    <mergeCell ref="AF26:AF27"/>
+    <mergeCell ref="AD17:AD18"/>
+    <mergeCell ref="AE17:AE18"/>
+    <mergeCell ref="AF17:AF18"/>
+    <mergeCell ref="AD19:AD20"/>
+    <mergeCell ref="AE19:AE20"/>
+    <mergeCell ref="AF19:AF20"/>
+    <mergeCell ref="AD24:AD25"/>
+    <mergeCell ref="AE24:AE25"/>
+    <mergeCell ref="AF24:AF25"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B1:R1"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="N26:N27"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="P26:P27"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="P24:P25"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="P15:P16"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="V26:V27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="B26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="Q26:Q27"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="V24:V25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="B24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="V19:V20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="P17:P18"/>
+    <mergeCell ref="V17:V18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="B15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="B13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="V15:V16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="Y13:Y14"/>
+    <mergeCell ref="Z13:Z14"/>
+    <mergeCell ref="AA13:AA14"/>
+    <mergeCell ref="AB13:AB14"/>
+    <mergeCell ref="AC13:AC14"/>
+    <mergeCell ref="AA17:AA18"/>
+    <mergeCell ref="AB17:AB18"/>
+    <mergeCell ref="AC17:AC18"/>
+    <mergeCell ref="X26:X27"/>
+    <mergeCell ref="Y26:Y27"/>
+    <mergeCell ref="Z26:Z27"/>
+    <mergeCell ref="AA26:AA27"/>
+    <mergeCell ref="AB26:AB27"/>
+    <mergeCell ref="AC26:AC27"/>
+    <mergeCell ref="AA19:AA20"/>
+    <mergeCell ref="AB19:AB20"/>
+    <mergeCell ref="AC19:AC20"/>
+    <mergeCell ref="AF13:AF14"/>
+    <mergeCell ref="AD15:AD16"/>
+    <mergeCell ref="W15:W16"/>
+    <mergeCell ref="W13:W14"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="X19:X20"/>
+    <mergeCell ref="W26:W27"/>
+    <mergeCell ref="W24:W25"/>
+    <mergeCell ref="X24:X25"/>
+    <mergeCell ref="Y24:Y25"/>
+    <mergeCell ref="Z24:Z25"/>
+    <mergeCell ref="Y19:Y20"/>
+    <mergeCell ref="Z19:Z20"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="W17:W18"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="X17:X18"/>
+    <mergeCell ref="Y17:Y18"/>
+    <mergeCell ref="Z17:Z18"/>
+    <mergeCell ref="AA24:AA25"/>
+    <mergeCell ref="AB24:AB25"/>
+    <mergeCell ref="AC24:AC25"/>
     <mergeCell ref="AE15:AE16"/>
     <mergeCell ref="AF15:AF16"/>
     <mergeCell ref="AA1:AC1"/>
@@ -3988,230 +4212,6 @@
     <mergeCell ref="AF2:AF3"/>
     <mergeCell ref="AD13:AD14"/>
     <mergeCell ref="AE13:AE14"/>
-    <mergeCell ref="AF13:AF14"/>
-    <mergeCell ref="AD15:AD16"/>
-    <mergeCell ref="W15:W16"/>
-    <mergeCell ref="W13:W14"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="X19:X20"/>
-    <mergeCell ref="W26:W27"/>
-    <mergeCell ref="W24:W25"/>
-    <mergeCell ref="X24:X25"/>
-    <mergeCell ref="Y24:Y25"/>
-    <mergeCell ref="Z24:Z25"/>
-    <mergeCell ref="Y19:Y20"/>
-    <mergeCell ref="Z19:Z20"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="W17:W18"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="X17:X18"/>
-    <mergeCell ref="Y17:Y18"/>
-    <mergeCell ref="Z17:Z18"/>
-    <mergeCell ref="AA24:AA25"/>
-    <mergeCell ref="AB24:AB25"/>
-    <mergeCell ref="AC24:AC25"/>
-    <mergeCell ref="X26:X27"/>
-    <mergeCell ref="Y26:Y27"/>
-    <mergeCell ref="Z26:Z27"/>
-    <mergeCell ref="AA26:AA27"/>
-    <mergeCell ref="AB26:AB27"/>
-    <mergeCell ref="AC26:AC27"/>
-    <mergeCell ref="AA19:AA20"/>
-    <mergeCell ref="AB19:AB20"/>
-    <mergeCell ref="AC19:AC20"/>
-    <mergeCell ref="X13:X14"/>
-    <mergeCell ref="Y13:Y14"/>
-    <mergeCell ref="Z13:Z14"/>
-    <mergeCell ref="AA13:AA14"/>
-    <mergeCell ref="AB13:AB14"/>
-    <mergeCell ref="AC13:AC14"/>
-    <mergeCell ref="AA17:AA18"/>
-    <mergeCell ref="AB17:AB18"/>
-    <mergeCell ref="AC17:AC18"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="V13:V14"/>
-    <mergeCell ref="B15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="B13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="V15:V16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="P17:P18"/>
-    <mergeCell ref="V17:V18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="V19:V20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="V24:V25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="V26:V27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="B26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="Q26:Q27"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B1:R1"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="N26:N27"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="P26:P27"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="P24:P25"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="P15:P16"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="AD26:AD27"/>
-    <mergeCell ref="AE26:AE27"/>
-    <mergeCell ref="AF26:AF27"/>
-    <mergeCell ref="AD17:AD18"/>
-    <mergeCell ref="AE17:AE18"/>
-    <mergeCell ref="AF17:AF18"/>
-    <mergeCell ref="AD19:AD20"/>
-    <mergeCell ref="AE19:AE20"/>
-    <mergeCell ref="AF19:AF20"/>
-    <mergeCell ref="AD24:AD25"/>
-    <mergeCell ref="AE24:AE25"/>
-    <mergeCell ref="AF24:AF25"/>
-    <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="R15:R16"/>
-    <mergeCell ref="R17:R18"/>
-    <mergeCell ref="R19:R20"/>
-    <mergeCell ref="Q15:Q16"/>
-    <mergeCell ref="Q17:Q18"/>
-    <mergeCell ref="Q19:Q20"/>
-    <mergeCell ref="Q24:Q25"/>
-    <mergeCell ref="R24:R25"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="U15:U16"/>
-    <mergeCell ref="U17:U18"/>
-    <mergeCell ref="U19:U20"/>
-    <mergeCell ref="U24:U25"/>
-    <mergeCell ref="U26:U27"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="S15:S16"/>
-    <mergeCell ref="S17:S18"/>
-    <mergeCell ref="S19:S20"/>
-    <mergeCell ref="S24:S25"/>
-    <mergeCell ref="S26:S27"/>
-    <mergeCell ref="T13:T14"/>
-    <mergeCell ref="T15:T16"/>
-    <mergeCell ref="T17:T18"/>
-    <mergeCell ref="T19:T20"/>
-    <mergeCell ref="T24:T25"/>
-    <mergeCell ref="T26:T27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
finished ALU not tested
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\CCE\Year 3 - Senior 1\Semester 2\Arch\Project\Repo\Architecture-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B09EECB-E24F-4A7C-BFB0-28F191512978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FB5B93-C1D5-4F7B-BFF3-F222F9E1C1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="390" windowWidth="25440" windowHeight="15390" xr2:uid="{0E858663-1FD8-418A-96F6-784D0D9CF43C}"/>
   </bookViews>
@@ -725,12 +725,54 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -743,50 +785,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1104,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9834DC43-CD6B-4773-9F5D-9D470392FD57}">
   <dimension ref="A1:BA40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AJ22" sqref="AJ22"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AH12" sqref="AH12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1146,25 +1146,25 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
+      <c r="B1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
       <c r="S1" s="22"/>
       <c r="T1" s="22"/>
       <c r="U1" s="22"/>
@@ -1174,21 +1174,21 @@
       <c r="W1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="X1" s="31" t="s">
+      <c r="X1" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="31" t="s">
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="31" t="s">
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
+      <c r="AE1" s="40"/>
+      <c r="AF1" s="40"/>
       <c r="AG1" s="13"/>
       <c r="AH1" s="14" t="s">
         <v>37</v>
@@ -1196,71 +1196,71 @@
       <c r="AI1" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="AK1" s="34" t="s">
+      <c r="AK1" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="AL1" s="35"/>
-      <c r="AM1" s="35"/>
-      <c r="AN1" s="36"/>
-      <c r="AP1" s="34" t="s">
+      <c r="AL1" s="49"/>
+      <c r="AM1" s="49"/>
+      <c r="AN1" s="50"/>
+      <c r="AP1" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="AQ1" s="35"/>
-      <c r="AR1" s="35"/>
-      <c r="AS1" s="36"/>
-      <c r="AU1" s="34" t="s">
+      <c r="AQ1" s="49"/>
+      <c r="AR1" s="49"/>
+      <c r="AS1" s="50"/>
+      <c r="AU1" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="AV1" s="35"/>
-      <c r="AW1" s="35"/>
-      <c r="AX1" s="36"/>
-      <c r="AZ1" s="34" t="s">
+      <c r="AV1" s="49"/>
+      <c r="AW1" s="49"/>
+      <c r="AX1" s="50"/>
+      <c r="AZ1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="BA1" s="35"/>
+      <c r="BA1" s="49"/>
     </row>
     <row r="2" spans="1:53" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="40" t="s">
+      <c r="C2" s="44"/>
+      <c r="D2" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="I2" s="40" t="s">
+      <c r="I2" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="40" t="s">
+      <c r="K2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="40" t="s">
+      <c r="L2" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="40" t="s">
+      <c r="M2" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="N2" s="40" t="s">
+      <c r="N2" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="O2" s="40" t="s">
+      <c r="O2" s="41" t="s">
         <v>11</v>
       </c>
       <c r="P2" s="29" t="s">
@@ -1348,11 +1348,11 @@
       <c r="AU2" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="AV2" s="37" t="s">
+      <c r="AV2" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="AW2" s="38"/>
-      <c r="AX2" s="39"/>
+      <c r="AW2" s="51"/>
+      <c r="AX2" s="34"/>
       <c r="AY2" s="16"/>
       <c r="AZ2" s="9" t="s">
         <v>98</v>
@@ -1363,20 +1363,20 @@
     </row>
     <row r="3" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="30"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
       <c r="P3" s="30"/>
       <c r="Q3" s="30"/>
       <c r="R3" s="30"/>
@@ -1406,10 +1406,10 @@
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="37">
-        <v>0</v>
-      </c>
-      <c r="C4" s="39"/>
+      <c r="B4" s="33">
+        <v>0</v>
+      </c>
+      <c r="C4" s="34"/>
       <c r="D4" s="2">
         <v>0</v>
       </c>
@@ -1489,10 +1489,10 @@
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="37">
-        <v>0</v>
-      </c>
-      <c r="C5" s="39"/>
+      <c r="B5" s="33">
+        <v>0</v>
+      </c>
+      <c r="C5" s="34"/>
       <c r="D5" s="2">
         <v>0</v>
       </c>
@@ -1572,10 +1572,10 @@
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="37">
-        <v>0</v>
-      </c>
-      <c r="C6" s="39"/>
+      <c r="B6" s="33">
+        <v>0</v>
+      </c>
+      <c r="C6" s="34"/>
       <c r="D6" s="2">
         <v>0</v>
       </c>
@@ -1663,10 +1663,10 @@
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="37">
-        <v>1</v>
-      </c>
-      <c r="C7" s="39"/>
+      <c r="B7" s="33">
+        <v>1</v>
+      </c>
+      <c r="C7" s="34"/>
       <c r="D7" s="2">
         <v>0</v>
       </c>
@@ -1754,10 +1754,10 @@
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="37">
-        <v>1</v>
-      </c>
-      <c r="C8" s="39"/>
+      <c r="B8" s="33">
+        <v>1</v>
+      </c>
+      <c r="C8" s="34"/>
       <c r="D8" s="2">
         <v>0</v>
       </c>
@@ -1845,10 +1845,10 @@
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="37">
-        <v>0</v>
-      </c>
-      <c r="C9" s="39"/>
+      <c r="B9" s="33">
+        <v>0</v>
+      </c>
+      <c r="C9" s="34"/>
       <c r="D9" s="2">
         <v>0</v>
       </c>
@@ -1936,10 +1936,10 @@
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="37">
-        <v>1</v>
-      </c>
-      <c r="C10" s="39"/>
+      <c r="B10" s="33">
+        <v>1</v>
+      </c>
+      <c r="C10" s="34"/>
       <c r="D10" s="2">
         <v>1</v>
       </c>
@@ -2027,10 +2027,10 @@
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="37">
-        <v>1</v>
-      </c>
-      <c r="C11" s="39"/>
+      <c r="B11" s="33">
+        <v>1</v>
+      </c>
+      <c r="C11" s="34"/>
       <c r="D11" s="2">
         <v>0</v>
       </c>
@@ -2118,10 +2118,10 @@
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="37">
-        <v>1</v>
-      </c>
-      <c r="C12" s="39"/>
+      <c r="B12" s="33">
+        <v>1</v>
+      </c>
+      <c r="C12" s="34"/>
       <c r="D12" s="2">
         <v>0</v>
       </c>
@@ -2206,13 +2206,13 @@
       </c>
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A13" s="50" t="s">
+      <c r="A13" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="46">
-        <v>1</v>
-      </c>
-      <c r="C13" s="47"/>
+      <c r="B13" s="35">
+        <v>1</v>
+      </c>
+      <c r="C13" s="36"/>
       <c r="D13" s="29">
         <v>0</v>
       </c>
@@ -2291,9 +2291,9 @@
       <c r="AG13" s="12"/>
     </row>
     <row r="14" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="51"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="49"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="38"/>
       <c r="D14" s="30"/>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
@@ -2326,13 +2326,13 @@
       <c r="AG14" s="12"/>
     </row>
     <row r="15" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="46">
-        <v>1</v>
-      </c>
-      <c r="C15" s="47"/>
+      <c r="B15" s="35">
+        <v>1</v>
+      </c>
+      <c r="C15" s="36"/>
       <c r="D15" s="29">
         <v>0</v>
       </c>
@@ -2411,9 +2411,9 @@
       <c r="AG15" s="12"/>
     </row>
     <row r="16" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="51"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="49"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38"/>
       <c r="D16" s="30"/>
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
@@ -2449,13 +2449,13 @@
       <c r="AK16" s="28"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="46">
-        <v>1</v>
-      </c>
-      <c r="C17" s="47"/>
+      <c r="B17" s="35">
+        <v>1</v>
+      </c>
+      <c r="C17" s="36"/>
       <c r="D17" s="29">
         <v>0</v>
       </c>
@@ -2534,9 +2534,9 @@
       <c r="AG17" s="12"/>
     </row>
     <row r="18" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="51"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="49"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="38"/>
       <c r="D18" s="30"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
@@ -2569,13 +2569,13 @@
       <c r="AG18" s="12"/>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="46">
-        <v>1</v>
-      </c>
-      <c r="C19" s="47"/>
+      <c r="B19" s="35">
+        <v>1</v>
+      </c>
+      <c r="C19" s="36"/>
       <c r="D19" s="29">
         <v>0</v>
       </c>
@@ -2654,9 +2654,9 @@
       <c r="AG19" s="12"/>
     </row>
     <row r="20" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="51"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="49"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="38"/>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
       <c r="F20" s="30"/>
@@ -2692,10 +2692,10 @@
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="37">
-        <v>0</v>
-      </c>
-      <c r="C21" s="39"/>
+      <c r="B21" s="33">
+        <v>0</v>
+      </c>
+      <c r="C21" s="34"/>
       <c r="D21" s="2">
         <v>0</v>
       </c>
@@ -2773,10 +2773,10 @@
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="37">
-        <v>1</v>
-      </c>
-      <c r="C22" s="39"/>
+      <c r="B22" s="33">
+        <v>1</v>
+      </c>
+      <c r="C22" s="34"/>
       <c r="D22" s="2">
         <v>0</v>
       </c>
@@ -2860,10 +2860,10 @@
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="37">
-        <v>1</v>
-      </c>
-      <c r="C23" s="39"/>
+      <c r="B23" s="33">
+        <v>1</v>
+      </c>
+      <c r="C23" s="34"/>
       <c r="D23" s="2">
         <v>0</v>
       </c>
@@ -2946,13 +2946,13 @@
       </c>
     </row>
     <row r="24" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="50" t="s">
+      <c r="A24" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="46">
-        <v>1</v>
-      </c>
-      <c r="C24" s="47"/>
+      <c r="B24" s="35">
+        <v>1</v>
+      </c>
+      <c r="C24" s="36"/>
       <c r="D24" s="29">
         <v>0</v>
       </c>
@@ -3037,9 +3037,9 @@
       </c>
     </row>
     <row r="25" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="51"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="49"/>
+      <c r="A25" s="32"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="38"/>
       <c r="D25" s="30"/>
       <c r="E25" s="30"/>
       <c r="F25" s="30"/>
@@ -3078,13 +3078,13 @@
       </c>
     </row>
     <row r="26" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="50" t="s">
+      <c r="A26" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="46">
-        <v>0</v>
-      </c>
-      <c r="C26" s="47"/>
+      <c r="B26" s="35">
+        <v>0</v>
+      </c>
+      <c r="C26" s="36"/>
       <c r="D26" s="29">
         <v>0</v>
       </c>
@@ -3169,9 +3169,9 @@
       </c>
     </row>
     <row r="27" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="51"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="49"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="38"/>
       <c r="D27" s="30"/>
       <c r="E27" s="30"/>
       <c r="F27" s="30"/>
@@ -3207,10 +3207,10 @@
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="37">
-        <v>0</v>
-      </c>
-      <c r="C28" s="39"/>
+      <c r="B28" s="33">
+        <v>0</v>
+      </c>
+      <c r="C28" s="34"/>
       <c r="D28" s="2">
         <v>0</v>
       </c>
@@ -3292,10 +3292,10 @@
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="37">
-        <v>0</v>
-      </c>
-      <c r="C29" s="39"/>
+      <c r="B29" s="33">
+        <v>0</v>
+      </c>
+      <c r="C29" s="34"/>
       <c r="D29" s="2">
         <v>0</v>
       </c>
@@ -3377,10 +3377,10 @@
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="37">
-        <v>0</v>
-      </c>
-      <c r="C30" s="39"/>
+      <c r="B30" s="33">
+        <v>0</v>
+      </c>
+      <c r="C30" s="34"/>
       <c r="D30" s="2">
         <v>0</v>
       </c>
@@ -3462,10 +3462,10 @@
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="37">
-        <v>0</v>
-      </c>
-      <c r="C31" s="39"/>
+      <c r="B31" s="33">
+        <v>0</v>
+      </c>
+      <c r="C31" s="34"/>
       <c r="D31" s="2">
         <v>0</v>
       </c>
@@ -3547,10 +3547,10 @@
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="37">
-        <v>0</v>
-      </c>
-      <c r="C32" s="39"/>
+      <c r="B32" s="33">
+        <v>0</v>
+      </c>
+      <c r="C32" s="34"/>
       <c r="D32" s="2">
         <v>0</v>
       </c>
@@ -3632,10 +3632,10 @@
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="37">
-        <v>0</v>
-      </c>
-      <c r="C33" s="39"/>
+      <c r="B33" s="33">
+        <v>0</v>
+      </c>
+      <c r="C33" s="34"/>
       <c r="D33" s="2">
         <v>0</v>
       </c>
@@ -3717,10 +3717,10 @@
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="37">
-        <v>0</v>
-      </c>
-      <c r="C34" s="39"/>
+      <c r="B34" s="33">
+        <v>0</v>
+      </c>
+      <c r="C34" s="34"/>
       <c r="D34" s="2">
         <v>0</v>
       </c>
@@ -3734,7 +3734,7 @@
         <v>4</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>69</v>
@@ -3802,10 +3802,10 @@
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="37">
-        <v>0</v>
-      </c>
-      <c r="C35" s="39"/>
+      <c r="B35" s="33">
+        <v>0</v>
+      </c>
+      <c r="C35" s="34"/>
       <c r="D35" s="2">
         <v>0</v>
       </c>
@@ -3894,8 +3894,8 @@
       <c r="A39" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="37"/>
-      <c r="C39" s="39"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="34"/>
       <c r="D39" s="21"/>
       <c r="E39" s="21"/>
       <c r="F39" s="21"/>
@@ -3930,8 +3930,8 @@
       <c r="A40" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="37"/>
-      <c r="C40" s="39"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="34"/>
       <c r="D40" s="23"/>
       <c r="E40" s="23"/>
       <c r="F40" s="23"/>
@@ -3964,56 +3964,180 @@
     </row>
   </sheetData>
   <mergeCells count="248">
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="U15:U16"/>
-    <mergeCell ref="U17:U18"/>
-    <mergeCell ref="U19:U20"/>
-    <mergeCell ref="U24:U25"/>
-    <mergeCell ref="U26:U27"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="S15:S16"/>
-    <mergeCell ref="S17:S18"/>
-    <mergeCell ref="S19:S20"/>
-    <mergeCell ref="S24:S25"/>
-    <mergeCell ref="S26:S27"/>
-    <mergeCell ref="T13:T14"/>
-    <mergeCell ref="T15:T16"/>
-    <mergeCell ref="T17:T18"/>
-    <mergeCell ref="T19:T20"/>
-    <mergeCell ref="T24:T25"/>
-    <mergeCell ref="T26:T27"/>
-    <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="R15:R16"/>
-    <mergeCell ref="R17:R18"/>
-    <mergeCell ref="R19:R20"/>
-    <mergeCell ref="Q15:Q16"/>
-    <mergeCell ref="Q17:Q18"/>
-    <mergeCell ref="Q19:Q20"/>
-    <mergeCell ref="Q24:Q25"/>
-    <mergeCell ref="R24:R25"/>
-    <mergeCell ref="AD26:AD27"/>
-    <mergeCell ref="AE26:AE27"/>
-    <mergeCell ref="AF26:AF27"/>
-    <mergeCell ref="AD17:AD18"/>
-    <mergeCell ref="AE17:AE18"/>
-    <mergeCell ref="AF17:AF18"/>
-    <mergeCell ref="AD19:AD20"/>
-    <mergeCell ref="AE19:AE20"/>
-    <mergeCell ref="AF19:AF20"/>
-    <mergeCell ref="AD24:AD25"/>
-    <mergeCell ref="AE24:AE25"/>
-    <mergeCell ref="AF24:AF25"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="AE15:AE16"/>
+    <mergeCell ref="AF15:AF16"/>
+    <mergeCell ref="AA1:AC1"/>
+    <mergeCell ref="X1:Z1"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="AZ1:BA1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AU1:AX1"/>
+    <mergeCell ref="X15:X16"/>
+    <mergeCell ref="Y15:Y16"/>
+    <mergeCell ref="Z15:Z16"/>
+    <mergeCell ref="AA15:AA16"/>
+    <mergeCell ref="AB15:AB16"/>
+    <mergeCell ref="AC15:AC16"/>
+    <mergeCell ref="AK1:AN1"/>
+    <mergeCell ref="AV2:AX2"/>
+    <mergeCell ref="AD1:AF1"/>
+    <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AD13:AD14"/>
+    <mergeCell ref="AE13:AE14"/>
+    <mergeCell ref="AF13:AF14"/>
+    <mergeCell ref="AD15:AD16"/>
+    <mergeCell ref="W15:W16"/>
+    <mergeCell ref="W13:W14"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="X19:X20"/>
+    <mergeCell ref="W26:W27"/>
+    <mergeCell ref="W24:W25"/>
+    <mergeCell ref="X24:X25"/>
+    <mergeCell ref="Y24:Y25"/>
+    <mergeCell ref="Z24:Z25"/>
+    <mergeCell ref="Y19:Y20"/>
+    <mergeCell ref="Z19:Z20"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="W17:W18"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="X17:X18"/>
+    <mergeCell ref="Y17:Y18"/>
+    <mergeCell ref="Z17:Z18"/>
+    <mergeCell ref="AA24:AA25"/>
+    <mergeCell ref="AB24:AB25"/>
+    <mergeCell ref="AC24:AC25"/>
+    <mergeCell ref="X26:X27"/>
+    <mergeCell ref="Y26:Y27"/>
+    <mergeCell ref="Z26:Z27"/>
+    <mergeCell ref="AA26:AA27"/>
+    <mergeCell ref="AB26:AB27"/>
+    <mergeCell ref="AC26:AC27"/>
+    <mergeCell ref="AA19:AA20"/>
+    <mergeCell ref="AB19:AB20"/>
+    <mergeCell ref="AC19:AC20"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="Y13:Y14"/>
+    <mergeCell ref="Z13:Z14"/>
+    <mergeCell ref="AA13:AA14"/>
+    <mergeCell ref="AB13:AB14"/>
+    <mergeCell ref="AC13:AC14"/>
+    <mergeCell ref="AA17:AA18"/>
+    <mergeCell ref="AB17:AB18"/>
+    <mergeCell ref="AC17:AC18"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="B15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="B13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="V15:V16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="P17:P18"/>
+    <mergeCell ref="V17:V18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="V19:V20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="V24:V25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="B24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="V26:V27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="B26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="Q26:Q27"/>
+    <mergeCell ref="R26:R27"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B1:R1"/>
     <mergeCell ref="B28:C28"/>
@@ -4038,180 +4162,56 @@
     <mergeCell ref="K15:K16"/>
     <mergeCell ref="L15:L16"/>
     <mergeCell ref="M17:M18"/>
-    <mergeCell ref="V26:V27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="B26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="Q26:Q27"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="V24:V25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="V19:V20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="P17:P18"/>
-    <mergeCell ref="V17:V18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="V13:V14"/>
-    <mergeCell ref="B15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="B13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="V15:V16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="X13:X14"/>
-    <mergeCell ref="Y13:Y14"/>
-    <mergeCell ref="Z13:Z14"/>
-    <mergeCell ref="AA13:AA14"/>
-    <mergeCell ref="AB13:AB14"/>
-    <mergeCell ref="AC13:AC14"/>
-    <mergeCell ref="AA17:AA18"/>
-    <mergeCell ref="AB17:AB18"/>
-    <mergeCell ref="AC17:AC18"/>
-    <mergeCell ref="X26:X27"/>
-    <mergeCell ref="Y26:Y27"/>
-    <mergeCell ref="Z26:Z27"/>
-    <mergeCell ref="AA26:AA27"/>
-    <mergeCell ref="AB26:AB27"/>
-    <mergeCell ref="AC26:AC27"/>
-    <mergeCell ref="AA19:AA20"/>
-    <mergeCell ref="AB19:AB20"/>
-    <mergeCell ref="AC19:AC20"/>
-    <mergeCell ref="AF13:AF14"/>
-    <mergeCell ref="AD15:AD16"/>
-    <mergeCell ref="W15:W16"/>
-    <mergeCell ref="W13:W14"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="X19:X20"/>
-    <mergeCell ref="W26:W27"/>
-    <mergeCell ref="W24:W25"/>
-    <mergeCell ref="X24:X25"/>
-    <mergeCell ref="Y24:Y25"/>
-    <mergeCell ref="Z24:Z25"/>
-    <mergeCell ref="Y19:Y20"/>
-    <mergeCell ref="Z19:Z20"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="W17:W18"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="X17:X18"/>
-    <mergeCell ref="Y17:Y18"/>
-    <mergeCell ref="Z17:Z18"/>
-    <mergeCell ref="AA24:AA25"/>
-    <mergeCell ref="AB24:AB25"/>
-    <mergeCell ref="AC24:AC25"/>
-    <mergeCell ref="AE15:AE16"/>
-    <mergeCell ref="AF15:AF16"/>
-    <mergeCell ref="AA1:AC1"/>
-    <mergeCell ref="X1:Z1"/>
-    <mergeCell ref="AA2:AA3"/>
-    <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="AZ1:BA1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AU1:AX1"/>
-    <mergeCell ref="X15:X16"/>
-    <mergeCell ref="Y15:Y16"/>
-    <mergeCell ref="Z15:Z16"/>
-    <mergeCell ref="AA15:AA16"/>
-    <mergeCell ref="AB15:AB16"/>
-    <mergeCell ref="AC15:AC16"/>
-    <mergeCell ref="AK1:AN1"/>
-    <mergeCell ref="AV2:AX2"/>
-    <mergeCell ref="AD1:AF1"/>
-    <mergeCell ref="AD2:AD3"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="AD13:AD14"/>
-    <mergeCell ref="AE13:AE14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="AD26:AD27"/>
+    <mergeCell ref="AE26:AE27"/>
+    <mergeCell ref="AF26:AF27"/>
+    <mergeCell ref="AD17:AD18"/>
+    <mergeCell ref="AE17:AE18"/>
+    <mergeCell ref="AF17:AF18"/>
+    <mergeCell ref="AD19:AD20"/>
+    <mergeCell ref="AE19:AE20"/>
+    <mergeCell ref="AF19:AF20"/>
+    <mergeCell ref="AD24:AD25"/>
+    <mergeCell ref="AE24:AE25"/>
+    <mergeCell ref="AF24:AF25"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="R15:R16"/>
+    <mergeCell ref="R17:R18"/>
+    <mergeCell ref="R19:R20"/>
+    <mergeCell ref="Q15:Q16"/>
+    <mergeCell ref="Q17:Q18"/>
+    <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="Q24:Q25"/>
+    <mergeCell ref="R24:R25"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="U15:U16"/>
+    <mergeCell ref="U17:U18"/>
+    <mergeCell ref="U19:U20"/>
+    <mergeCell ref="U24:U25"/>
+    <mergeCell ref="U26:U27"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="S15:S16"/>
+    <mergeCell ref="S17:S18"/>
+    <mergeCell ref="S19:S20"/>
+    <mergeCell ref="S24:S25"/>
+    <mergeCell ref="S26:S27"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="T15:T16"/>
+    <mergeCell ref="T17:T18"/>
+    <mergeCell ref="T19:T20"/>
+    <mergeCell ref="T24:T25"/>
+    <mergeCell ref="T26:T27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed One Operand Bugs
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\CCE\Year 3 - Senior 1\Semester 2\Arch\Project\Repo\Architecture-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CCE\Semester 8\Computer Architecture\Project\Architecture-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F200C07-6CB5-4337-BB7F-05C7EF264172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8892A49-1C73-49E4-A63C-D19A84A07E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0E858663-1FD8-418A-96F6-784D0D9CF43C}"/>
   </bookViews>
@@ -781,7 +781,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -886,70 +886,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -958,10 +901,70 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1278,10 +1281,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9834DC43-CD6B-4773-9F5D-9D470392FD57}">
-  <dimension ref="A1:BC40"/>
+  <dimension ref="A1:BD40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1334,185 +1337,186 @@
     <col min="54" max="54" width="23.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" ht="83.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:56" ht="83.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
+      <c r="B1" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
       <c r="S1" s="21"/>
       <c r="T1" s="21"/>
       <c r="U1" s="21"/>
-      <c r="V1" s="13" t="s">
+      <c r="V1" s="36"/>
+      <c r="W1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="X1" s="45" t="s">
+      <c r="Y1" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="45" t="s">
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="41" t="s">
+      <c r="AC1" s="50"/>
+      <c r="AD1" s="50"/>
+      <c r="AE1" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="AE1" s="42"/>
-      <c r="AF1" s="43"/>
-      <c r="AG1" s="28" t="s">
+      <c r="AF1" s="60"/>
+      <c r="AG1" s="61"/>
+      <c r="AH1" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="AH1" s="12"/>
-      <c r="AJ1" s="13" t="s">
+      <c r="AI1" s="12"/>
+      <c r="AK1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="AK1" s="29" t="s">
+      <c r="AL1" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="AM1" s="30" t="s">
+      <c r="AN1" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="AN1" s="31"/>
       <c r="AO1" s="31"/>
-      <c r="AP1" s="32"/>
-      <c r="AR1" s="30" t="s">
+      <c r="AP1" s="31"/>
+      <c r="AQ1" s="32"/>
+      <c r="AS1" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="AS1" s="31"/>
       <c r="AT1" s="31"/>
-      <c r="AU1" s="32"/>
-      <c r="AW1" s="30" t="s">
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="32"/>
+      <c r="AX1" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="AX1" s="31"/>
       <c r="AY1" s="31"/>
-      <c r="AZ1" s="32"/>
-      <c r="BB1" s="30" t="s">
+      <c r="AZ1" s="31"/>
+      <c r="BA1" s="32"/>
+      <c r="BC1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="BC1" s="31"/>
+      <c r="BD1" s="31"/>
     </row>
-    <row r="2" spans="1:55" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="36" t="s">
+    <row r="2" spans="1:56" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="53" t="s">
         <v>141</v>
       </c>
-      <c r="D2" s="51"/>
-      <c r="E2" s="48" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="51" t="s">
         <v>140</v>
       </c>
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="51" t="s">
         <v>139</v>
       </c>
-      <c r="G2" s="48" t="s">
+      <c r="G2" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="I2" s="48" t="s">
+      <c r="I2" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="J2" s="48" t="s">
+      <c r="J2" s="51" t="s">
         <v>135</v>
       </c>
-      <c r="K2" s="48" t="s">
+      <c r="K2" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="L2" s="48" t="s">
+      <c r="L2" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="M2" s="48" t="s">
+      <c r="M2" s="51" t="s">
         <v>132</v>
       </c>
-      <c r="N2" s="48" t="s">
+      <c r="N2" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="O2" s="48" t="s">
+      <c r="O2" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="P2" s="48" t="s">
+      <c r="P2" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="Q2" s="36" t="s">
+      <c r="Q2" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="R2" s="36" t="s">
+      <c r="R2" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="S2" s="36" t="s">
+      <c r="S2" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="T2" s="36" t="s">
+      <c r="T2" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="U2" s="36" t="s">
+      <c r="U2" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="V2" s="36" t="s">
+      <c r="V2" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="W2" s="36" t="s">
+      <c r="W2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="X2" s="36" t="s">
+      <c r="X2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="Y2" s="36" t="s">
+      <c r="Y2" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="Z2" s="36" t="s">
+      <c r="Z2" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="AA2" s="36" t="s">
+      <c r="AA2" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="AB2" s="36" t="s">
+      <c r="AB2" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="AC2" s="36" t="s">
+      <c r="AC2" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="AD2" s="36" t="s">
+      <c r="AD2" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="AE2" s="44" t="s">
+      <c r="AE2" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="AF2" s="44" t="s">
+      <c r="AF2" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="AG2" s="44" t="s">
+      <c r="AG2" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="AH2" s="44" t="s">
+      <c r="AH2" s="62" t="s">
         <v>4</v>
       </c>
       <c r="AI2" s="12"/>
@@ -1549,11 +1553,11 @@
       <c r="AW2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="AX2" s="38" t="s">
+      <c r="AX2" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="AY2" s="39"/>
-      <c r="AZ2" s="40"/>
+      <c r="AY2" s="58"/>
+      <c r="AZ2" s="42"/>
       <c r="BA2" s="15"/>
       <c r="BB2" s="9" t="s">
         <v>88</v>
@@ -1562,41 +1566,41 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="37"/>
-      <c r="AB3" s="37"/>
-      <c r="AC3" s="37"/>
-      <c r="AD3" s="37"/>
-      <c r="AE3" s="37"/>
-      <c r="AF3" s="37"/>
-      <c r="AG3" s="37"/>
-      <c r="AH3" s="37"/>
+    <row r="3" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
+      <c r="V3" s="38"/>
+      <c r="W3" s="38"/>
+      <c r="X3" s="38"/>
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="38"/>
+      <c r="AB3" s="38"/>
+      <c r="AC3" s="38"/>
+      <c r="AD3" s="38"/>
+      <c r="AE3" s="38"/>
+      <c r="AF3" s="38"/>
+      <c r="AG3" s="38"/>
+      <c r="AH3" s="38"/>
       <c r="AI3" s="12"/>
       <c r="AJ3" s="14" t="s">
         <v>31</v>
@@ -1605,17 +1609,17 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:55" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:56" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="34">
         <v>0</v>
       </c>
-      <c r="C4" s="38">
-        <v>0</v>
-      </c>
-      <c r="D4" s="40"/>
+      <c r="C4" s="41">
+        <v>0</v>
+      </c>
+      <c r="D4" s="42"/>
       <c r="E4" s="2">
         <v>0</v>
       </c>
@@ -1694,17 +1698,17 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:55" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:56" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="34">
         <v>0</v>
       </c>
-      <c r="C5" s="38">
-        <v>0</v>
-      </c>
-      <c r="D5" s="40"/>
+      <c r="C5" s="41">
+        <v>0</v>
+      </c>
+      <c r="D5" s="42"/>
       <c r="E5" s="2">
         <v>0</v>
       </c>
@@ -1783,17 +1787,17 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:55" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:56" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="34">
         <v>0</v>
       </c>
-      <c r="C6" s="38">
-        <v>0</v>
-      </c>
-      <c r="D6" s="40"/>
+      <c r="C6" s="41">
+        <v>0</v>
+      </c>
+      <c r="D6" s="42"/>
       <c r="E6" s="2">
         <v>0</v>
       </c>
@@ -1880,17 +1884,17 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:55" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:56" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="34">
         <v>0</v>
       </c>
-      <c r="C7" s="38">
-        <v>1</v>
-      </c>
-      <c r="D7" s="40"/>
+      <c r="C7" s="41">
+        <v>1</v>
+      </c>
+      <c r="D7" s="42"/>
       <c r="E7" s="2">
         <v>0</v>
       </c>
@@ -1977,17 +1981,17 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:55" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:56" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="34">
         <v>0</v>
       </c>
-      <c r="C8" s="38">
-        <v>1</v>
-      </c>
-      <c r="D8" s="40"/>
+      <c r="C8" s="41">
+        <v>1</v>
+      </c>
+      <c r="D8" s="42"/>
       <c r="E8" s="2">
         <v>0</v>
       </c>
@@ -2074,17 +2078,17 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:55" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:56" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="34">
         <v>0</v>
       </c>
-      <c r="C9" s="38">
-        <v>0</v>
-      </c>
-      <c r="D9" s="40"/>
+      <c r="C9" s="41">
+        <v>0</v>
+      </c>
+      <c r="D9" s="42"/>
       <c r="E9" s="2">
         <v>0</v>
       </c>
@@ -2171,17 +2175,17 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:55" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:56" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="34">
         <v>0</v>
       </c>
-      <c r="C10" s="38">
-        <v>1</v>
-      </c>
-      <c r="D10" s="40"/>
+      <c r="C10" s="41">
+        <v>1</v>
+      </c>
+      <c r="D10" s="42"/>
       <c r="E10" s="2">
         <v>1</v>
       </c>
@@ -2268,17 +2272,17 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:55" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:56" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="34">
         <v>0</v>
       </c>
-      <c r="C11" s="38">
-        <v>1</v>
-      </c>
-      <c r="D11" s="40"/>
+      <c r="C11" s="41">
+        <v>1</v>
+      </c>
+      <c r="D11" s="42"/>
       <c r="E11" s="2">
         <v>0</v>
       </c>
@@ -2365,17 +2369,17 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:55" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:56" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="34">
         <v>0</v>
       </c>
-      <c r="C12" s="38">
-        <v>1</v>
-      </c>
-      <c r="D12" s="40"/>
+      <c r="C12" s="41">
+        <v>1</v>
+      </c>
+      <c r="D12" s="42"/>
       <c r="E12" s="2">
         <v>0</v>
       </c>
@@ -2462,519 +2466,519 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:55" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="58" t="s">
+    <row r="13" spans="1:56" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="60">
-        <v>0</v>
-      </c>
-      <c r="C13" s="54">
-        <v>1</v>
-      </c>
-      <c r="D13" s="55"/>
-      <c r="E13" s="36">
-        <v>0</v>
-      </c>
-      <c r="F13" s="36">
-        <v>0</v>
-      </c>
-      <c r="G13" s="36">
-        <v>0</v>
-      </c>
-      <c r="H13" s="36" t="s">
+      <c r="B13" s="47">
+        <v>0</v>
+      </c>
+      <c r="C13" s="43">
+        <v>1</v>
+      </c>
+      <c r="D13" s="44"/>
+      <c r="E13" s="37">
+        <v>0</v>
+      </c>
+      <c r="F13" s="37">
+        <v>0</v>
+      </c>
+      <c r="G13" s="37">
+        <v>0</v>
+      </c>
+      <c r="H13" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="I13" s="36" t="s">
+      <c r="I13" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="J13" s="36" t="s">
+      <c r="J13" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="K13" s="36">
-        <v>0</v>
-      </c>
-      <c r="L13" s="36">
-        <v>0</v>
-      </c>
-      <c r="M13" s="36">
-        <v>0</v>
-      </c>
-      <c r="N13" s="36">
-        <v>0</v>
-      </c>
-      <c r="O13" s="36">
-        <v>0</v>
-      </c>
-      <c r="P13" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="36">
-        <v>0</v>
-      </c>
-      <c r="R13" s="36">
-        <v>0</v>
-      </c>
-      <c r="S13" s="36">
-        <v>0</v>
-      </c>
-      <c r="T13" s="36">
-        <v>0</v>
-      </c>
-      <c r="U13" s="36">
-        <v>0</v>
-      </c>
-      <c r="V13" s="36">
-        <v>0</v>
-      </c>
-      <c r="W13" s="36" t="s">
+      <c r="K13" s="37">
+        <v>0</v>
+      </c>
+      <c r="L13" s="37">
+        <v>0</v>
+      </c>
+      <c r="M13" s="37">
+        <v>0</v>
+      </c>
+      <c r="N13" s="37">
+        <v>0</v>
+      </c>
+      <c r="O13" s="37">
+        <v>0</v>
+      </c>
+      <c r="P13" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="37">
+        <v>0</v>
+      </c>
+      <c r="R13" s="37">
+        <v>0</v>
+      </c>
+      <c r="S13" s="37">
+        <v>0</v>
+      </c>
+      <c r="T13" s="37">
+        <v>0</v>
+      </c>
+      <c r="U13" s="37">
+        <v>0</v>
+      </c>
+      <c r="V13" s="37">
+        <v>0</v>
+      </c>
+      <c r="W13" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="X13" s="36" t="s">
+      <c r="X13" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="Y13" s="36" t="s">
+      <c r="Y13" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="Z13" s="36" t="s">
+      <c r="Z13" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="AA13" s="36" t="s">
+      <c r="AA13" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="AB13" s="36"/>
-      <c r="AC13" s="36"/>
-      <c r="AD13" s="36"/>
-      <c r="AE13" s="36"/>
-      <c r="AF13" s="36"/>
-      <c r="AG13" s="36"/>
-      <c r="AH13" s="36" t="s">
+      <c r="AB13" s="37"/>
+      <c r="AC13" s="37"/>
+      <c r="AD13" s="37"/>
+      <c r="AE13" s="37"/>
+      <c r="AF13" s="37"/>
+      <c r="AG13" s="37"/>
+      <c r="AH13" s="37" t="s">
         <v>150</v>
       </c>
       <c r="AI13" s="11"/>
     </row>
-    <row r="14" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="59"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="37"/>
-      <c r="R14" s="37"/>
-      <c r="S14" s="37"/>
-      <c r="T14" s="37"/>
-      <c r="U14" s="37"/>
-      <c r="V14" s="37"/>
-      <c r="W14" s="37"/>
-      <c r="X14" s="37"/>
-      <c r="Y14" s="37"/>
-      <c r="Z14" s="37"/>
-      <c r="AA14" s="37"/>
-      <c r="AB14" s="37"/>
-      <c r="AC14" s="37"/>
-      <c r="AD14" s="37"/>
-      <c r="AE14" s="37"/>
-      <c r="AF14" s="37"/>
-      <c r="AG14" s="37"/>
-      <c r="AH14" s="37"/>
+    <row r="14" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="40"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="38"/>
+      <c r="R14" s="38"/>
+      <c r="S14" s="38"/>
+      <c r="T14" s="38"/>
+      <c r="U14" s="38"/>
+      <c r="V14" s="38"/>
+      <c r="W14" s="38"/>
+      <c r="X14" s="38"/>
+      <c r="Y14" s="38"/>
+      <c r="Z14" s="38"/>
+      <c r="AA14" s="38"/>
+      <c r="AB14" s="38"/>
+      <c r="AC14" s="38"/>
+      <c r="AD14" s="38"/>
+      <c r="AE14" s="38"/>
+      <c r="AF14" s="38"/>
+      <c r="AG14" s="38"/>
+      <c r="AH14" s="38"/>
       <c r="AI14" s="11"/>
     </row>
-    <row r="15" spans="1:55" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="58" t="s">
+    <row r="15" spans="1:56" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="60">
-        <v>0</v>
-      </c>
-      <c r="C15" s="54">
-        <v>1</v>
-      </c>
-      <c r="D15" s="55"/>
-      <c r="E15" s="36">
-        <v>0</v>
-      </c>
-      <c r="F15" s="36">
-        <v>0</v>
-      </c>
-      <c r="G15" s="36">
-        <v>0</v>
-      </c>
-      <c r="H15" s="36" t="s">
+      <c r="B15" s="47">
+        <v>0</v>
+      </c>
+      <c r="C15" s="43">
+        <v>1</v>
+      </c>
+      <c r="D15" s="44"/>
+      <c r="E15" s="37">
+        <v>0</v>
+      </c>
+      <c r="F15" s="37">
+        <v>0</v>
+      </c>
+      <c r="G15" s="37">
+        <v>0</v>
+      </c>
+      <c r="H15" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="I15" s="36" t="s">
+      <c r="I15" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="J15" s="36" t="s">
+      <c r="J15" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="K15" s="36">
-        <v>0</v>
-      </c>
-      <c r="L15" s="36">
-        <v>0</v>
-      </c>
-      <c r="M15" s="36">
-        <v>0</v>
-      </c>
-      <c r="N15" s="36">
-        <v>0</v>
-      </c>
-      <c r="O15" s="36">
-        <v>0</v>
-      </c>
-      <c r="P15" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="36">
-        <v>0</v>
-      </c>
-      <c r="R15" s="36">
-        <v>0</v>
-      </c>
-      <c r="S15" s="36">
-        <v>0</v>
-      </c>
-      <c r="T15" s="36">
-        <v>0</v>
-      </c>
-      <c r="U15" s="36">
-        <v>0</v>
-      </c>
-      <c r="V15" s="36">
-        <v>0</v>
-      </c>
-      <c r="W15" s="36" t="s">
+      <c r="K15" s="37">
+        <v>0</v>
+      </c>
+      <c r="L15" s="37">
+        <v>0</v>
+      </c>
+      <c r="M15" s="37">
+        <v>0</v>
+      </c>
+      <c r="N15" s="37">
+        <v>0</v>
+      </c>
+      <c r="O15" s="37">
+        <v>0</v>
+      </c>
+      <c r="P15" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="37">
+        <v>0</v>
+      </c>
+      <c r="R15" s="37">
+        <v>0</v>
+      </c>
+      <c r="S15" s="37">
+        <v>0</v>
+      </c>
+      <c r="T15" s="37">
+        <v>0</v>
+      </c>
+      <c r="U15" s="37">
+        <v>0</v>
+      </c>
+      <c r="V15" s="37">
+        <v>0</v>
+      </c>
+      <c r="W15" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="X15" s="36" t="s">
+      <c r="X15" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="Y15" s="36" t="s">
+      <c r="Y15" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="Z15" s="36" t="s">
+      <c r="Z15" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="AA15" s="36" t="s">
+      <c r="AA15" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="AB15" s="36"/>
-      <c r="AC15" s="36"/>
-      <c r="AD15" s="36"/>
-      <c r="AE15" s="36"/>
-      <c r="AF15" s="36"/>
-      <c r="AG15" s="36"/>
-      <c r="AH15" s="36" t="s">
+      <c r="AB15" s="37"/>
+      <c r="AC15" s="37"/>
+      <c r="AD15" s="37"/>
+      <c r="AE15" s="37"/>
+      <c r="AF15" s="37"/>
+      <c r="AG15" s="37"/>
+      <c r="AH15" s="37" t="s">
         <v>151</v>
       </c>
       <c r="AI15" s="11"/>
     </row>
-    <row r="16" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="59"/>
-      <c r="B16" s="61"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="37"/>
-      <c r="N16" s="37"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="37"/>
-      <c r="Q16" s="37"/>
-      <c r="R16" s="37"/>
-      <c r="S16" s="37"/>
-      <c r="T16" s="37"/>
-      <c r="U16" s="37"/>
-      <c r="V16" s="37"/>
-      <c r="W16" s="37"/>
-      <c r="X16" s="37"/>
-      <c r="Y16" s="37"/>
-      <c r="Z16" s="37"/>
-      <c r="AA16" s="37"/>
-      <c r="AB16" s="37"/>
-      <c r="AC16" s="37"/>
-      <c r="AD16" s="37"/>
-      <c r="AE16" s="37"/>
-      <c r="AF16" s="37"/>
-      <c r="AG16" s="37"/>
-      <c r="AH16" s="37"/>
+    <row r="16" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="40"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="38"/>
+      <c r="Q16" s="38"/>
+      <c r="R16" s="38"/>
+      <c r="S16" s="38"/>
+      <c r="T16" s="38"/>
+      <c r="U16" s="38"/>
+      <c r="V16" s="38"/>
+      <c r="W16" s="38"/>
+      <c r="X16" s="38"/>
+      <c r="Y16" s="38"/>
+      <c r="Z16" s="38"/>
+      <c r="AA16" s="38"/>
+      <c r="AB16" s="38"/>
+      <c r="AC16" s="38"/>
+      <c r="AD16" s="38"/>
+      <c r="AE16" s="38"/>
+      <c r="AF16" s="38"/>
+      <c r="AG16" s="38"/>
+      <c r="AH16" s="38"/>
       <c r="AI16" s="11"/>
       <c r="AK16" s="26"/>
       <c r="AL16" s="11"/>
       <c r="AM16" s="27"/>
     </row>
     <row r="17" spans="1:37" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="58" t="s">
+      <c r="A17" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="60">
-        <v>0</v>
-      </c>
-      <c r="C17" s="54">
-        <v>1</v>
-      </c>
-      <c r="D17" s="55"/>
-      <c r="E17" s="36">
-        <v>0</v>
-      </c>
-      <c r="F17" s="36">
-        <v>0</v>
-      </c>
-      <c r="G17" s="36">
-        <v>0</v>
-      </c>
-      <c r="H17" s="36" t="s">
+      <c r="B17" s="47">
+        <v>0</v>
+      </c>
+      <c r="C17" s="43">
+        <v>1</v>
+      </c>
+      <c r="D17" s="44"/>
+      <c r="E17" s="37">
+        <v>0</v>
+      </c>
+      <c r="F17" s="37">
+        <v>0</v>
+      </c>
+      <c r="G17" s="37">
+        <v>0</v>
+      </c>
+      <c r="H17" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="I17" s="36" t="s">
+      <c r="I17" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="J17" s="36" t="s">
+      <c r="J17" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="K17" s="36">
-        <v>0</v>
-      </c>
-      <c r="L17" s="36">
-        <v>0</v>
-      </c>
-      <c r="M17" s="36">
-        <v>0</v>
-      </c>
-      <c r="N17" s="36">
-        <v>0</v>
-      </c>
-      <c r="O17" s="36">
-        <v>0</v>
-      </c>
-      <c r="P17" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="36">
-        <v>0</v>
-      </c>
-      <c r="R17" s="36">
-        <v>0</v>
-      </c>
-      <c r="S17" s="36">
-        <v>0</v>
-      </c>
-      <c r="T17" s="36">
-        <v>0</v>
-      </c>
-      <c r="U17" s="36">
-        <v>0</v>
-      </c>
-      <c r="V17" s="36">
-        <v>0</v>
-      </c>
-      <c r="W17" s="36" t="s">
+      <c r="K17" s="37">
+        <v>0</v>
+      </c>
+      <c r="L17" s="37">
+        <v>0</v>
+      </c>
+      <c r="M17" s="37">
+        <v>0</v>
+      </c>
+      <c r="N17" s="37">
+        <v>0</v>
+      </c>
+      <c r="O17" s="37">
+        <v>0</v>
+      </c>
+      <c r="P17" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="37">
+        <v>0</v>
+      </c>
+      <c r="R17" s="37">
+        <v>0</v>
+      </c>
+      <c r="S17" s="37">
+        <v>0</v>
+      </c>
+      <c r="T17" s="37">
+        <v>0</v>
+      </c>
+      <c r="U17" s="37">
+        <v>0</v>
+      </c>
+      <c r="V17" s="37">
+        <v>0</v>
+      </c>
+      <c r="W17" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="X17" s="36" t="s">
+      <c r="X17" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="Y17" s="36" t="s">
+      <c r="Y17" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="Z17" s="36" t="s">
+      <c r="Z17" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="AA17" s="36" t="s">
+      <c r="AA17" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="AB17" s="36"/>
-      <c r="AC17" s="36"/>
-      <c r="AD17" s="36"/>
-      <c r="AE17" s="36"/>
-      <c r="AF17" s="36"/>
-      <c r="AG17" s="36"/>
-      <c r="AH17" s="36" t="s">
+      <c r="AB17" s="37"/>
+      <c r="AC17" s="37"/>
+      <c r="AD17" s="37"/>
+      <c r="AE17" s="37"/>
+      <c r="AF17" s="37"/>
+      <c r="AG17" s="37"/>
+      <c r="AH17" s="37" t="s">
         <v>152</v>
       </c>
       <c r="AI17" s="11"/>
     </row>
     <row r="18" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="59"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="37"/>
-      <c r="R18" s="37"/>
-      <c r="S18" s="37"/>
-      <c r="T18" s="37"/>
-      <c r="U18" s="37"/>
-      <c r="V18" s="37"/>
-      <c r="W18" s="37"/>
-      <c r="X18" s="37"/>
-      <c r="Y18" s="37"/>
-      <c r="Z18" s="37"/>
-      <c r="AA18" s="37"/>
-      <c r="AB18" s="37"/>
-      <c r="AC18" s="37"/>
-      <c r="AD18" s="37"/>
-      <c r="AE18" s="37"/>
-      <c r="AF18" s="37"/>
-      <c r="AG18" s="37"/>
-      <c r="AH18" s="37"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="38"/>
+      <c r="R18" s="38"/>
+      <c r="S18" s="38"/>
+      <c r="T18" s="38"/>
+      <c r="U18" s="38"/>
+      <c r="V18" s="38"/>
+      <c r="W18" s="38"/>
+      <c r="X18" s="38"/>
+      <c r="Y18" s="38"/>
+      <c r="Z18" s="38"/>
+      <c r="AA18" s="38"/>
+      <c r="AB18" s="38"/>
+      <c r="AC18" s="38"/>
+      <c r="AD18" s="38"/>
+      <c r="AE18" s="38"/>
+      <c r="AF18" s="38"/>
+      <c r="AG18" s="38"/>
+      <c r="AH18" s="38"/>
       <c r="AI18" s="11"/>
     </row>
     <row r="19" spans="1:37" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="60">
-        <v>0</v>
-      </c>
-      <c r="C19" s="54">
-        <v>1</v>
-      </c>
-      <c r="D19" s="55"/>
-      <c r="E19" s="36">
-        <v>0</v>
-      </c>
-      <c r="F19" s="36">
-        <v>0</v>
-      </c>
-      <c r="G19" s="36">
-        <v>1</v>
-      </c>
-      <c r="H19" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="I19" s="36" t="s">
+      <c r="B19" s="47">
+        <v>0</v>
+      </c>
+      <c r="C19" s="43">
+        <v>1</v>
+      </c>
+      <c r="D19" s="44"/>
+      <c r="E19" s="37">
+        <v>0</v>
+      </c>
+      <c r="F19" s="37">
+        <v>0</v>
+      </c>
+      <c r="G19" s="37">
+        <v>1</v>
+      </c>
+      <c r="H19" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="I19" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="J19" s="36" t="s">
+      <c r="J19" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="K19" s="36">
-        <v>0</v>
-      </c>
-      <c r="L19" s="36">
-        <v>0</v>
-      </c>
-      <c r="M19" s="36">
-        <v>0</v>
-      </c>
-      <c r="N19" s="36">
-        <v>0</v>
-      </c>
-      <c r="O19" s="36">
-        <v>0</v>
-      </c>
-      <c r="P19" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="36">
-        <v>0</v>
-      </c>
-      <c r="R19" s="36">
-        <v>0</v>
-      </c>
-      <c r="S19" s="36">
-        <v>0</v>
-      </c>
-      <c r="T19" s="36">
-        <v>0</v>
-      </c>
-      <c r="U19" s="36">
-        <v>0</v>
-      </c>
-      <c r="V19" s="36">
-        <v>0</v>
-      </c>
-      <c r="W19" s="36" t="s">
+      <c r="K19" s="37">
+        <v>0</v>
+      </c>
+      <c r="L19" s="37">
+        <v>0</v>
+      </c>
+      <c r="M19" s="37">
+        <v>0</v>
+      </c>
+      <c r="N19" s="37">
+        <v>0</v>
+      </c>
+      <c r="O19" s="37">
+        <v>0</v>
+      </c>
+      <c r="P19" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="37">
+        <v>0</v>
+      </c>
+      <c r="R19" s="37">
+        <v>0</v>
+      </c>
+      <c r="S19" s="37">
+        <v>0</v>
+      </c>
+      <c r="T19" s="37">
+        <v>0</v>
+      </c>
+      <c r="U19" s="37">
+        <v>0</v>
+      </c>
+      <c r="V19" s="37">
+        <v>0</v>
+      </c>
+      <c r="W19" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="X19" s="36" t="s">
+      <c r="X19" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="Y19" s="36"/>
-      <c r="Z19" s="36"/>
-      <c r="AA19" s="36"/>
-      <c r="AB19" s="36" t="s">
+      <c r="Y19" s="37"/>
+      <c r="Z19" s="37"/>
+      <c r="AA19" s="37"/>
+      <c r="AB19" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="AC19" s="36" t="s">
+      <c r="AC19" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="AD19" s="36" t="s">
+      <c r="AD19" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="AE19" s="36"/>
-      <c r="AF19" s="36"/>
-      <c r="AG19" s="36"/>
-      <c r="AH19" s="36" t="s">
+      <c r="AE19" s="37"/>
+      <c r="AF19" s="37"/>
+      <c r="AG19" s="37"/>
+      <c r="AH19" s="37" t="s">
         <v>153</v>
       </c>
       <c r="AI19" s="11"/>
     </row>
     <row r="20" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="59"/>
-      <c r="B20" s="61"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="37"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="37"/>
-      <c r="Q20" s="37"/>
-      <c r="R20" s="37"/>
-      <c r="S20" s="37"/>
-      <c r="T20" s="37"/>
-      <c r="U20" s="37"/>
-      <c r="V20" s="37"/>
-      <c r="W20" s="37"/>
-      <c r="X20" s="37"/>
-      <c r="Y20" s="37"/>
-      <c r="Z20" s="37"/>
-      <c r="AA20" s="37"/>
-      <c r="AB20" s="37"/>
-      <c r="AC20" s="37"/>
-      <c r="AD20" s="37"/>
-      <c r="AE20" s="37"/>
-      <c r="AF20" s="37"/>
-      <c r="AG20" s="37"/>
-      <c r="AH20" s="37"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="38"/>
+      <c r="R20" s="38"/>
+      <c r="S20" s="38"/>
+      <c r="T20" s="38"/>
+      <c r="U20" s="38"/>
+      <c r="V20" s="38"/>
+      <c r="W20" s="38"/>
+      <c r="X20" s="38"/>
+      <c r="Y20" s="38"/>
+      <c r="Z20" s="38"/>
+      <c r="AA20" s="38"/>
+      <c r="AB20" s="38"/>
+      <c r="AC20" s="38"/>
+      <c r="AD20" s="38"/>
+      <c r="AE20" s="38"/>
+      <c r="AF20" s="38"/>
+      <c r="AG20" s="38"/>
+      <c r="AH20" s="38"/>
       <c r="AI20" s="11"/>
     </row>
     <row r="21" spans="1:37" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2984,10 +2988,10 @@
       <c r="B21" s="34">
         <v>0</v>
       </c>
-      <c r="C21" s="38">
-        <v>0</v>
-      </c>
-      <c r="D21" s="40"/>
+      <c r="C21" s="41">
+        <v>0</v>
+      </c>
+      <c r="D21" s="42"/>
       <c r="E21" s="2">
         <v>0</v>
       </c>
@@ -3071,10 +3075,10 @@
       <c r="B22" s="34">
         <v>0</v>
       </c>
-      <c r="C22" s="38">
-        <v>1</v>
-      </c>
-      <c r="D22" s="40"/>
+      <c r="C22" s="41">
+        <v>1</v>
+      </c>
+      <c r="D22" s="42"/>
       <c r="E22" s="2">
         <v>0</v>
       </c>
@@ -3164,10 +3168,10 @@
       <c r="B23" s="34">
         <v>0</v>
       </c>
-      <c r="C23" s="38">
-        <v>1</v>
-      </c>
-      <c r="D23" s="40"/>
+      <c r="C23" s="41">
+        <v>1</v>
+      </c>
+      <c r="D23" s="42"/>
       <c r="E23" s="2">
         <v>0</v>
       </c>
@@ -3253,92 +3257,92 @@
       </c>
     </row>
     <row r="24" spans="1:37" ht="45.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="58" t="s">
+      <c r="A24" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="60">
-        <v>0</v>
-      </c>
-      <c r="C24" s="54">
-        <v>1</v>
-      </c>
-      <c r="D24" s="55"/>
-      <c r="E24" s="36">
-        <v>0</v>
-      </c>
-      <c r="F24" s="36">
-        <v>0</v>
-      </c>
-      <c r="G24" s="36">
-        <v>1</v>
-      </c>
-      <c r="H24" s="36" t="s">
+      <c r="B24" s="47">
+        <v>0</v>
+      </c>
+      <c r="C24" s="43">
+        <v>1</v>
+      </c>
+      <c r="D24" s="44"/>
+      <c r="E24" s="37">
+        <v>0</v>
+      </c>
+      <c r="F24" s="37">
+        <v>0</v>
+      </c>
+      <c r="G24" s="37">
+        <v>1</v>
+      </c>
+      <c r="H24" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="I24" s="36" t="s">
+      <c r="I24" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="J24" s="36" t="s">
+      <c r="J24" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="K24" s="36">
-        <v>0</v>
-      </c>
-      <c r="L24" s="36">
-        <v>0</v>
-      </c>
-      <c r="M24" s="36">
-        <v>0</v>
-      </c>
-      <c r="N24" s="36">
-        <v>1</v>
-      </c>
-      <c r="O24" s="36">
-        <v>1</v>
-      </c>
-      <c r="P24" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="36">
-        <v>0</v>
-      </c>
-      <c r="R24" s="36">
-        <v>0</v>
-      </c>
-      <c r="S24" s="36">
-        <v>0</v>
-      </c>
-      <c r="T24" s="36">
-        <v>0</v>
-      </c>
-      <c r="U24" s="36">
-        <v>0</v>
-      </c>
-      <c r="V24" s="36">
-        <v>0</v>
-      </c>
-      <c r="W24" s="36" t="s">
+      <c r="K24" s="37">
+        <v>0</v>
+      </c>
+      <c r="L24" s="37">
+        <v>0</v>
+      </c>
+      <c r="M24" s="37">
+        <v>0</v>
+      </c>
+      <c r="N24" s="37">
+        <v>1</v>
+      </c>
+      <c r="O24" s="37">
+        <v>1</v>
+      </c>
+      <c r="P24" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="37">
+        <v>0</v>
+      </c>
+      <c r="R24" s="37">
+        <v>0</v>
+      </c>
+      <c r="S24" s="37">
+        <v>0</v>
+      </c>
+      <c r="T24" s="37">
+        <v>0</v>
+      </c>
+      <c r="U24" s="37">
+        <v>0</v>
+      </c>
+      <c r="V24" s="37">
+        <v>0</v>
+      </c>
+      <c r="W24" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="X24" s="36" t="s">
+      <c r="X24" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="Y24" s="36"/>
-      <c r="Z24" s="36"/>
-      <c r="AA24" s="36"/>
-      <c r="AB24" s="36" t="s">
+      <c r="Y24" s="37"/>
+      <c r="Z24" s="37"/>
+      <c r="AA24" s="37"/>
+      <c r="AB24" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="AC24" s="36" t="s">
+      <c r="AC24" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="AD24" s="36" t="s">
+      <c r="AD24" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="AE24" s="36"/>
-      <c r="AF24" s="36"/>
-      <c r="AG24" s="36"/>
-      <c r="AH24" s="36" t="s">
+      <c r="AE24" s="37"/>
+      <c r="AF24" s="37"/>
+      <c r="AG24" s="37"/>
+      <c r="AH24" s="37" t="s">
         <v>158</v>
       </c>
       <c r="AI24" s="11"/>
@@ -3350,40 +3354,40 @@
       </c>
     </row>
     <row r="25" spans="1:37" ht="34.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="59"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="37"/>
-      <c r="L25" s="37"/>
-      <c r="M25" s="37"/>
-      <c r="N25" s="37"/>
-      <c r="O25" s="37"/>
-      <c r="P25" s="37"/>
-      <c r="Q25" s="37"/>
-      <c r="R25" s="37"/>
-      <c r="S25" s="37"/>
-      <c r="T25" s="37"/>
-      <c r="U25" s="37"/>
-      <c r="V25" s="37"/>
-      <c r="W25" s="37"/>
-      <c r="X25" s="37"/>
-      <c r="Y25" s="37"/>
-      <c r="Z25" s="37"/>
-      <c r="AA25" s="37"/>
-      <c r="AB25" s="37"/>
-      <c r="AC25" s="37"/>
-      <c r="AD25" s="37"/>
-      <c r="AE25" s="37"/>
-      <c r="AF25" s="37"/>
-      <c r="AG25" s="37"/>
-      <c r="AH25" s="37"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="38"/>
+      <c r="S25" s="38"/>
+      <c r="T25" s="38"/>
+      <c r="U25" s="38"/>
+      <c r="V25" s="38"/>
+      <c r="W25" s="38"/>
+      <c r="X25" s="38"/>
+      <c r="Y25" s="38"/>
+      <c r="Z25" s="38"/>
+      <c r="AA25" s="38"/>
+      <c r="AB25" s="38"/>
+      <c r="AC25" s="38"/>
+      <c r="AD25" s="38"/>
+      <c r="AE25" s="38"/>
+      <c r="AF25" s="38"/>
+      <c r="AG25" s="38"/>
+      <c r="AH25" s="38"/>
       <c r="AI25" s="11"/>
       <c r="AJ25" s="14" t="s">
         <v>94</v>
@@ -3393,92 +3397,92 @@
       </c>
     </row>
     <row r="26" spans="1:37" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="58" t="s">
+      <c r="A26" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="60">
-        <v>0</v>
-      </c>
-      <c r="C26" s="54">
-        <v>0</v>
-      </c>
-      <c r="D26" s="55"/>
-      <c r="E26" s="36">
-        <v>0</v>
-      </c>
-      <c r="F26" s="36">
-        <v>0</v>
-      </c>
-      <c r="G26" s="36">
-        <v>1</v>
-      </c>
-      <c r="H26" s="36" t="s">
+      <c r="B26" s="47">
+        <v>0</v>
+      </c>
+      <c r="C26" s="43">
+        <v>0</v>
+      </c>
+      <c r="D26" s="44"/>
+      <c r="E26" s="37">
+        <v>0</v>
+      </c>
+      <c r="F26" s="37">
+        <v>0</v>
+      </c>
+      <c r="G26" s="37">
+        <v>1</v>
+      </c>
+      <c r="H26" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="I26" s="36" t="s">
+      <c r="I26" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="J26" s="36" t="s">
+      <c r="J26" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="K26" s="36">
-        <v>0</v>
-      </c>
-      <c r="L26" s="36">
-        <v>0</v>
-      </c>
-      <c r="M26" s="36">
-        <v>1</v>
-      </c>
-      <c r="N26" s="36">
-        <v>0</v>
-      </c>
-      <c r="O26" s="36" t="s">
+      <c r="K26" s="37">
+        <v>0</v>
+      </c>
+      <c r="L26" s="37">
+        <v>0</v>
+      </c>
+      <c r="M26" s="37">
+        <v>1</v>
+      </c>
+      <c r="N26" s="37">
+        <v>0</v>
+      </c>
+      <c r="O26" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="P26" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="36">
-        <v>0</v>
-      </c>
-      <c r="R26" s="36">
-        <v>0</v>
-      </c>
-      <c r="S26" s="36">
-        <v>0</v>
-      </c>
-      <c r="T26" s="36">
-        <v>0</v>
-      </c>
-      <c r="U26" s="36">
-        <v>0</v>
-      </c>
-      <c r="V26" s="36">
-        <v>0</v>
-      </c>
-      <c r="W26" s="36" t="s">
+      <c r="P26" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="37">
+        <v>0</v>
+      </c>
+      <c r="R26" s="37">
+        <v>0</v>
+      </c>
+      <c r="S26" s="37">
+        <v>0</v>
+      </c>
+      <c r="T26" s="37">
+        <v>0</v>
+      </c>
+      <c r="U26" s="37">
+        <v>0</v>
+      </c>
+      <c r="V26" s="37">
+        <v>0</v>
+      </c>
+      <c r="W26" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="X26" s="36" t="s">
+      <c r="X26" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="Y26" s="36"/>
-      <c r="Z26" s="36"/>
-      <c r="AA26" s="36"/>
-      <c r="AB26" s="36" t="s">
+      <c r="Y26" s="37"/>
+      <c r="Z26" s="37"/>
+      <c r="AA26" s="37"/>
+      <c r="AB26" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="AC26" s="36" t="s">
+      <c r="AC26" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="AD26" s="36" t="s">
+      <c r="AD26" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="AE26" s="36"/>
-      <c r="AF26" s="36"/>
-      <c r="AG26" s="36"/>
-      <c r="AH26" s="36" t="s">
+      <c r="AE26" s="37"/>
+      <c r="AF26" s="37"/>
+      <c r="AG26" s="37"/>
+      <c r="AH26" s="37" t="s">
         <v>157</v>
       </c>
       <c r="AI26" s="11"/>
@@ -3490,40 +3494,40 @@
       </c>
     </row>
     <row r="27" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="59"/>
-      <c r="B27" s="61"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="37"/>
-      <c r="M27" s="37"/>
-      <c r="N27" s="37"/>
-      <c r="O27" s="37"/>
-      <c r="P27" s="37"/>
-      <c r="Q27" s="37"/>
-      <c r="R27" s="37"/>
-      <c r="S27" s="37"/>
-      <c r="T27" s="37"/>
-      <c r="U27" s="37"/>
-      <c r="V27" s="37"/>
-      <c r="W27" s="37"/>
-      <c r="X27" s="37"/>
-      <c r="Y27" s="37"/>
-      <c r="Z27" s="37"/>
-      <c r="AA27" s="37"/>
-      <c r="AB27" s="37"/>
-      <c r="AC27" s="37"/>
-      <c r="AD27" s="37"/>
-      <c r="AE27" s="37"/>
-      <c r="AF27" s="37"/>
-      <c r="AG27" s="37"/>
-      <c r="AH27" s="37"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="38"/>
+      <c r="P27" s="38"/>
+      <c r="Q27" s="38"/>
+      <c r="R27" s="38"/>
+      <c r="S27" s="38"/>
+      <c r="T27" s="38"/>
+      <c r="U27" s="38"/>
+      <c r="V27" s="38"/>
+      <c r="W27" s="38"/>
+      <c r="X27" s="38"/>
+      <c r="Y27" s="38"/>
+      <c r="Z27" s="38"/>
+      <c r="AA27" s="38"/>
+      <c r="AB27" s="38"/>
+      <c r="AC27" s="38"/>
+      <c r="AD27" s="38"/>
+      <c r="AE27" s="38"/>
+      <c r="AF27" s="38"/>
+      <c r="AG27" s="38"/>
+      <c r="AH27" s="38"/>
       <c r="AI27" s="11"/>
     </row>
     <row r="28" spans="1:37" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3533,10 +3537,10 @@
       <c r="B28" s="34">
         <v>0</v>
       </c>
-      <c r="C28" s="38">
-        <v>0</v>
-      </c>
-      <c r="D28" s="40"/>
+      <c r="C28" s="41">
+        <v>0</v>
+      </c>
+      <c r="D28" s="42"/>
       <c r="E28" s="2">
         <v>0</v>
       </c>
@@ -3624,10 +3628,10 @@
       <c r="B29" s="34">
         <v>0</v>
       </c>
-      <c r="C29" s="38">
-        <v>0</v>
-      </c>
-      <c r="D29" s="40"/>
+      <c r="C29" s="41">
+        <v>0</v>
+      </c>
+      <c r="D29" s="42"/>
       <c r="E29" s="2">
         <v>0</v>
       </c>
@@ -3715,10 +3719,10 @@
       <c r="B30" s="34">
         <v>0</v>
       </c>
-      <c r="C30" s="38">
-        <v>0</v>
-      </c>
-      <c r="D30" s="40"/>
+      <c r="C30" s="41">
+        <v>0</v>
+      </c>
+      <c r="D30" s="42"/>
       <c r="E30" s="2">
         <v>0</v>
       </c>
@@ -3806,10 +3810,10 @@
       <c r="B31" s="34">
         <v>0</v>
       </c>
-      <c r="C31" s="38">
-        <v>0</v>
-      </c>
-      <c r="D31" s="40"/>
+      <c r="C31" s="41">
+        <v>0</v>
+      </c>
+      <c r="D31" s="42"/>
       <c r="E31" s="2">
         <v>0</v>
       </c>
@@ -3897,10 +3901,10 @@
       <c r="B32" s="34">
         <v>0</v>
       </c>
-      <c r="C32" s="38">
-        <v>0</v>
-      </c>
-      <c r="D32" s="40"/>
+      <c r="C32" s="41">
+        <v>0</v>
+      </c>
+      <c r="D32" s="42"/>
       <c r="E32" s="2">
         <v>0</v>
       </c>
@@ -3988,10 +3992,10 @@
       <c r="B33" s="34">
         <v>0</v>
       </c>
-      <c r="C33" s="38">
-        <v>0</v>
-      </c>
-      <c r="D33" s="40"/>
+      <c r="C33" s="41">
+        <v>0</v>
+      </c>
+      <c r="D33" s="42"/>
       <c r="E33" s="2">
         <v>0</v>
       </c>
@@ -4079,10 +4083,10 @@
       <c r="B34" s="34">
         <v>0</v>
       </c>
-      <c r="C34" s="38">
-        <v>0</v>
-      </c>
-      <c r="D34" s="40"/>
+      <c r="C34" s="41">
+        <v>0</v>
+      </c>
+      <c r="D34" s="42"/>
       <c r="E34" s="2">
         <v>0</v>
       </c>
@@ -4170,10 +4174,10 @@
       <c r="B35" s="34">
         <v>0</v>
       </c>
-      <c r="C35" s="38">
-        <v>0</v>
-      </c>
-      <c r="D35" s="40"/>
+      <c r="C35" s="41">
+        <v>0</v>
+      </c>
+      <c r="D35" s="42"/>
       <c r="E35" s="2">
         <v>0</v>
       </c>
@@ -4266,8 +4270,8 @@
         <v>28</v>
       </c>
       <c r="B39" s="33"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="40"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="42"/>
       <c r="E39" s="20"/>
       <c r="F39" s="20"/>
       <c r="G39" s="20"/>
@@ -4306,10 +4310,10 @@
       <c r="B40" s="34">
         <v>1</v>
       </c>
-      <c r="C40" s="38">
-        <v>0</v>
-      </c>
-      <c r="D40" s="40"/>
+      <c r="C40" s="41">
+        <v>0</v>
+      </c>
+      <c r="D40" s="42"/>
       <c r="E40" s="22">
         <v>0</v>
       </c>
@@ -4383,52 +4387,171 @@
     </row>
   </sheetData>
   <mergeCells count="258">
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="U15:U16"/>
-    <mergeCell ref="U17:U18"/>
-    <mergeCell ref="U19:U20"/>
-    <mergeCell ref="U24:U25"/>
-    <mergeCell ref="U26:U27"/>
-    <mergeCell ref="AE19:AE20"/>
-    <mergeCell ref="AF19:AF20"/>
-    <mergeCell ref="AG19:AG20"/>
-    <mergeCell ref="AE24:AE25"/>
-    <mergeCell ref="AF24:AF25"/>
-    <mergeCell ref="AG24:AG25"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="S15:S16"/>
-    <mergeCell ref="S17:S18"/>
-    <mergeCell ref="S19:S20"/>
-    <mergeCell ref="R15:R16"/>
-    <mergeCell ref="R17:R18"/>
-    <mergeCell ref="R19:R20"/>
-    <mergeCell ref="R24:R25"/>
-    <mergeCell ref="S24:S25"/>
-    <mergeCell ref="V13:V14"/>
-    <mergeCell ref="V15:V16"/>
-    <mergeCell ref="V17:V18"/>
-    <mergeCell ref="V19:V20"/>
-    <mergeCell ref="V24:V25"/>
-    <mergeCell ref="T13:T14"/>
-    <mergeCell ref="T15:T16"/>
-    <mergeCell ref="T17:T18"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C17:D18"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="AH17:AH18"/>
+    <mergeCell ref="AH19:AH20"/>
+    <mergeCell ref="AH24:AH25"/>
+    <mergeCell ref="AH26:AH27"/>
+    <mergeCell ref="AF15:AF16"/>
+    <mergeCell ref="AG15:AG16"/>
+    <mergeCell ref="AX2:AZ2"/>
+    <mergeCell ref="AE1:AG1"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="AE13:AE14"/>
+    <mergeCell ref="AF13:AF14"/>
+    <mergeCell ref="AG13:AG14"/>
+    <mergeCell ref="AE15:AE16"/>
+    <mergeCell ref="AH2:AH3"/>
+    <mergeCell ref="AH13:AH14"/>
+    <mergeCell ref="AH15:AH16"/>
+    <mergeCell ref="AE26:AE27"/>
+    <mergeCell ref="AF26:AF27"/>
+    <mergeCell ref="AG26:AG27"/>
+    <mergeCell ref="AE17:AE18"/>
+    <mergeCell ref="AF17:AF18"/>
+    <mergeCell ref="AG17:AG18"/>
+    <mergeCell ref="AB1:AD1"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="Y15:Y16"/>
+    <mergeCell ref="Z15:Z16"/>
+    <mergeCell ref="AA15:AA16"/>
+    <mergeCell ref="AB15:AB16"/>
+    <mergeCell ref="AC15:AC16"/>
+    <mergeCell ref="AD15:AD16"/>
+    <mergeCell ref="X15:X16"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="X26:X27"/>
+    <mergeCell ref="X24:X25"/>
+    <mergeCell ref="Y24:Y25"/>
+    <mergeCell ref="Z24:Z25"/>
+    <mergeCell ref="AA24:AA25"/>
+    <mergeCell ref="Z19:Z20"/>
+    <mergeCell ref="AA19:AA20"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="X17:X18"/>
+    <mergeCell ref="X19:X20"/>
+    <mergeCell ref="Y17:Y18"/>
+    <mergeCell ref="Z17:Z18"/>
+    <mergeCell ref="AA17:AA18"/>
+    <mergeCell ref="AB24:AB25"/>
+    <mergeCell ref="AC24:AC25"/>
+    <mergeCell ref="AD24:AD25"/>
+    <mergeCell ref="Y26:Y27"/>
+    <mergeCell ref="Z26:Z27"/>
+    <mergeCell ref="AA26:AA27"/>
+    <mergeCell ref="AB26:AB27"/>
+    <mergeCell ref="AC26:AC27"/>
+    <mergeCell ref="AD26:AD27"/>
+    <mergeCell ref="AD19:AD20"/>
+    <mergeCell ref="Y13:Y14"/>
+    <mergeCell ref="Z13:Z14"/>
+    <mergeCell ref="AA13:AA14"/>
+    <mergeCell ref="AB13:AB14"/>
+    <mergeCell ref="AC13:AC14"/>
+    <mergeCell ref="AD13:AD14"/>
+    <mergeCell ref="AB17:AB18"/>
+    <mergeCell ref="AC17:AC18"/>
+    <mergeCell ref="AD17:AD18"/>
+    <mergeCell ref="Y19:Y20"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="C2:D3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="P17:P18"/>
+    <mergeCell ref="Q17:Q18"/>
+    <mergeCell ref="W17:W18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="T24:T25"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="C19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="T19:T20"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="B1:R1"/>
     <mergeCell ref="C28:D28"/>
@@ -4453,194 +4576,75 @@
     <mergeCell ref="L15:L16"/>
     <mergeCell ref="M15:M16"/>
     <mergeCell ref="N17:N18"/>
-    <mergeCell ref="W26:W27"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C17:D18"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C26:D27"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="T15:T16"/>
+    <mergeCell ref="T17:T18"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="I26:I27"/>
     <mergeCell ref="J26:J27"/>
     <mergeCell ref="K26:K27"/>
     <mergeCell ref="L26:L27"/>
     <mergeCell ref="M26:M27"/>
     <mergeCell ref="N26:N27"/>
-    <mergeCell ref="C26:D27"/>
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="F26:F27"/>
     <mergeCell ref="G26:G27"/>
     <mergeCell ref="H26:H27"/>
     <mergeCell ref="R26:R27"/>
     <mergeCell ref="S26:S27"/>
+    <mergeCell ref="T26:T27"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="S15:S16"/>
+    <mergeCell ref="S17:S18"/>
+    <mergeCell ref="S19:S20"/>
+    <mergeCell ref="R15:R16"/>
+    <mergeCell ref="R17:R18"/>
+    <mergeCell ref="R19:R20"/>
+    <mergeCell ref="R24:R25"/>
+    <mergeCell ref="S24:S25"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="U15:U16"/>
+    <mergeCell ref="U17:U18"/>
+    <mergeCell ref="U19:U20"/>
+    <mergeCell ref="U24:U25"/>
+    <mergeCell ref="U26:U27"/>
+    <mergeCell ref="AE19:AE20"/>
+    <mergeCell ref="AF19:AF20"/>
+    <mergeCell ref="AG19:AG20"/>
+    <mergeCell ref="AE24:AE25"/>
+    <mergeCell ref="AF24:AF25"/>
+    <mergeCell ref="AG24:AG25"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="V15:V16"/>
+    <mergeCell ref="V17:V18"/>
+    <mergeCell ref="V19:V20"/>
+    <mergeCell ref="V24:V25"/>
+    <mergeCell ref="W26:W27"/>
     <mergeCell ref="V26:V27"/>
-    <mergeCell ref="T26:T27"/>
     <mergeCell ref="W24:W25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="C24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="T24:T25"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="Q19:Q20"/>
-    <mergeCell ref="C19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="T19:T20"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="P17:P18"/>
-    <mergeCell ref="Q17:Q18"/>
-    <mergeCell ref="W17:W18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="O17:O18"/>
     <mergeCell ref="W13:W14"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="E13:E14"/>
     <mergeCell ref="W15:W16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="C2:D3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="B2:B3"/>
     <mergeCell ref="AB19:AB20"/>
     <mergeCell ref="AC19:AC20"/>
-    <mergeCell ref="AD19:AD20"/>
-    <mergeCell ref="Y13:Y14"/>
-    <mergeCell ref="Z13:Z14"/>
-    <mergeCell ref="AA13:AA14"/>
-    <mergeCell ref="AB13:AB14"/>
-    <mergeCell ref="AC13:AC14"/>
-    <mergeCell ref="AD13:AD14"/>
-    <mergeCell ref="AB17:AB18"/>
-    <mergeCell ref="AC17:AC18"/>
-    <mergeCell ref="AD17:AD18"/>
-    <mergeCell ref="AB24:AB25"/>
-    <mergeCell ref="AC24:AC25"/>
-    <mergeCell ref="AD24:AD25"/>
-    <mergeCell ref="Y26:Y27"/>
-    <mergeCell ref="Z26:Z27"/>
-    <mergeCell ref="AA26:AA27"/>
-    <mergeCell ref="AB26:AB27"/>
-    <mergeCell ref="AC26:AC27"/>
-    <mergeCell ref="AD26:AD27"/>
-    <mergeCell ref="Y19:Y20"/>
-    <mergeCell ref="X26:X27"/>
-    <mergeCell ref="X24:X25"/>
-    <mergeCell ref="Y24:Y25"/>
-    <mergeCell ref="Z24:Z25"/>
-    <mergeCell ref="AA24:AA25"/>
-    <mergeCell ref="Z19:Z20"/>
-    <mergeCell ref="AA19:AA20"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="AA2:AA3"/>
-    <mergeCell ref="X17:X18"/>
-    <mergeCell ref="X19:X20"/>
-    <mergeCell ref="Y17:Y18"/>
-    <mergeCell ref="Z17:Z18"/>
-    <mergeCell ref="AA17:AA18"/>
-    <mergeCell ref="AA1:AC1"/>
-    <mergeCell ref="X1:Z1"/>
-    <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="AD2:AD3"/>
-    <mergeCell ref="Y15:Y16"/>
-    <mergeCell ref="Z15:Z16"/>
-    <mergeCell ref="AA15:AA16"/>
-    <mergeCell ref="AB15:AB16"/>
-    <mergeCell ref="AC15:AC16"/>
-    <mergeCell ref="AD15:AD16"/>
-    <mergeCell ref="X15:X16"/>
-    <mergeCell ref="X13:X14"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="AH17:AH18"/>
-    <mergeCell ref="AH19:AH20"/>
-    <mergeCell ref="AH24:AH25"/>
-    <mergeCell ref="AH26:AH27"/>
-    <mergeCell ref="AF15:AF16"/>
-    <mergeCell ref="AG15:AG16"/>
-    <mergeCell ref="AX2:AZ2"/>
-    <mergeCell ref="AD1:AF1"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AE13:AE14"/>
-    <mergeCell ref="AF13:AF14"/>
-    <mergeCell ref="AG13:AG14"/>
-    <mergeCell ref="AE15:AE16"/>
-    <mergeCell ref="AH2:AH3"/>
-    <mergeCell ref="AH13:AH14"/>
-    <mergeCell ref="AH15:AH16"/>
-    <mergeCell ref="AE26:AE27"/>
-    <mergeCell ref="AF26:AF27"/>
-    <mergeCell ref="AG26:AG27"/>
-    <mergeCell ref="AE17:AE18"/>
-    <mergeCell ref="AF17:AF18"/>
-    <mergeCell ref="AG17:AG18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>